<commit_message>
NOT ADDING 1ST-LEVEL UPDATES TO SIMI FROM THIS COMMIT ONWARDS!
1. Implemented x-standardisation if wanted to dlc.
=>  Automatically generates x-standardised df & XLS file
=> Normalised df automatically based on x-standardised steps
=> Thus also average & std dfs
=> Plots automatically based on non-x-standardised SCs for individual SC-level plots (#1-5) or on standardised SCs in average plots (#6 onwards)

2. Fixed tests accordingly
=> Had to update approval test files since new columns are added
=> New unit test to check that angles do not depend on x-standardisation

3. Y-standardisation can now be performed with reference to a joint of choice (previously was based on global y-minimum)

4. (x/y) Standardisation operations were renamed from "Normalised". I renamed this to avoid confusion to "Normalised Stepcycles" which is based on SCs being equally long so we can compute averages
</commit_message>
<xml_diff>
--- a/tests/test_data/dlc_data/true_data/ID 12 - Run 3 - Average Stepcycle.xlsx
+++ b/tests/test_data/dlc_data/true_data/ID 12 - Run 3 - Average Stepcycle.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX26"/>
+  <dimension ref="A1:BJ26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -684,97 +684,157 @@
           <t>Hip Angle Acceleration</t>
         </is>
       </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>Ankle Angle Velocity Velocity</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>Ankle Angle Velocity Acceleration</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>Ankle Angle Acceleration Velocity</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>Ankle Angle Acceleration Acceleration</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>Knee Angle Velocity Velocity</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>Knee Angle Velocity Acceleration</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>Knee Angle Acceleration Velocity</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>Knee Angle Acceleration Acceleration</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>Hip Angle Velocity Velocity</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>Hip Angle Velocity Acceleration</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>Hip Angle Acceleration Velocity</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>Hip Angle Acceleration Acceleration</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>219.6082274964515</v>
+        <v>92.78763887730051</v>
       </c>
       <c r="C2" t="n">
         <v>6.957703448356462</v>
       </c>
       <c r="D2" t="n">
-        <v>205.7424803997608</v>
+        <v>78.92189178060977</v>
       </c>
       <c r="E2" t="n">
         <v>18.05841161849651</v>
       </c>
       <c r="F2" t="n">
-        <v>190.2895815829013</v>
+        <v>63.4689929637503</v>
       </c>
       <c r="G2" t="n">
         <v>2.795020570146278</v>
       </c>
       <c r="H2" t="n">
-        <v>185.4243795922463</v>
+        <v>58.60379097309522</v>
       </c>
       <c r="I2" t="n">
         <v>4.668385931786069</v>
       </c>
       <c r="J2" t="n">
-        <v>182.9140095000572</v>
+        <v>56.09342088090614</v>
       </c>
       <c r="K2" t="n">
         <v>15.77499470812209</v>
       </c>
       <c r="L2" t="n">
-        <v>191.8037576878325</v>
+        <v>64.98316906868145</v>
       </c>
       <c r="M2" t="n">
         <v>19.28525478281874</v>
       </c>
       <c r="N2" t="n">
-        <v>188.0774213912639</v>
+        <v>61.25683277211288</v>
       </c>
       <c r="O2" t="n">
         <v>27.50478298106092</v>
       </c>
       <c r="P2" t="n">
-        <v>141.6901446403341</v>
+        <v>14.86955602118309</v>
       </c>
       <c r="Q2" t="n">
         <v>27.26243607541348</v>
       </c>
       <c r="R2" t="n">
-        <v>136.5561931691271</v>
+        <v>9.735604549976095</v>
       </c>
       <c r="S2" t="n">
         <v>21.05782691468584</v>
       </c>
       <c r="T2" t="n">
-        <v>141.4119274058241</v>
+        <v>14.59133878667305</v>
       </c>
       <c r="U2" t="n">
         <v>13.36871613847449</v>
       </c>
       <c r="V2" t="n">
-        <v>129.764427022731</v>
+        <v>2.943838403580024</v>
       </c>
       <c r="W2" t="n">
         <v>16.84982624459774</v>
       </c>
       <c r="X2" t="n">
-        <v>129.1749873059861</v>
+        <v>2.354398686835097</v>
       </c>
       <c r="Y2" t="n">
         <v>4.651759533171955</v>
       </c>
       <c r="Z2" t="n">
-        <v>125.6416077309467</v>
+        <v>-1.17898088820435</v>
       </c>
       <c r="AA2" t="n">
         <v>21.05383365712267</v>
       </c>
       <c r="AB2" t="n">
-        <v>93.0503195904671</v>
+        <v>-33.77026902868392</v>
       </c>
       <c r="AC2" t="n">
         <v>33.96507425511138</v>
       </c>
       <c r="AD2" t="n">
-        <v>67.55681545176405</v>
+        <v>-59.26377316738697</v>
       </c>
       <c r="AE2" t="n">
         <v>39.30151919101147</v>
@@ -835,6 +895,42 @@
       </c>
       <c r="AX2" t="n">
         <v>1.598217427140197</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>1.530466154794912</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>-1.773557206108463</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>-1.773557206108463</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0.8686249019213583</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>7.246022910409843</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0.3261180542288133</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0.3261180542288133</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>-1.478764311488017</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>1.598217427140197</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>1.128723850572865</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>1.128723850572865</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>-0.9391337800894628</v>
       </c>
     </row>
     <row r="3">
@@ -842,91 +938,91 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>222.0471118358856</v>
+        <v>95.22652321673455</v>
       </c>
       <c r="C3" t="n">
         <v>6.994072934414476</v>
       </c>
       <c r="D3" t="n">
-        <v>207.9148794742341</v>
+        <v>81.09429085508305</v>
       </c>
       <c r="E3" t="n">
         <v>17.9234078589906</v>
       </c>
       <c r="F3" t="n">
-        <v>190.7654904304667</v>
+        <v>63.94490181131566</v>
       </c>
       <c r="G3" t="n">
         <v>2.939747749490941</v>
       </c>
       <c r="H3" t="n">
-        <v>185.6693693932067</v>
+        <v>58.84878077405568</v>
       </c>
       <c r="I3" t="n">
         <v>4.543044719290222</v>
       </c>
       <c r="J3" t="n">
-        <v>184.5703642419044</v>
+        <v>57.7497756227534</v>
       </c>
       <c r="K3" t="n">
         <v>15.60487950101811</v>
       </c>
       <c r="L3" t="n">
-        <v>193.5133000637623</v>
+        <v>66.69271144461126</v>
       </c>
       <c r="M3" t="n">
         <v>19.23161364616232</v>
       </c>
       <c r="N3" t="n">
-        <v>189.801102496208</v>
+        <v>62.980513877057</v>
       </c>
       <c r="O3" t="n">
         <v>27.59978517572931</v>
       </c>
       <c r="P3" t="n">
-        <v>143.7586885817508</v>
+        <v>16.93809996259975</v>
       </c>
       <c r="Q3" t="n">
         <v>27.28565297228226</v>
       </c>
       <c r="R3" t="n">
-        <v>139.2169992974464</v>
+        <v>12.39641067829537</v>
       </c>
       <c r="S3" t="n">
         <v>20.9976115125291</v>
       </c>
       <c r="T3" t="n">
-        <v>146.5961030189027</v>
+        <v>19.77551439975171</v>
       </c>
       <c r="U3" t="n">
         <v>15.42572670794549</v>
       </c>
       <c r="V3" t="n">
-        <v>134.6126556396484</v>
+        <v>7.792067020497399</v>
       </c>
       <c r="W3" t="n">
         <v>16.15057194486578</v>
       </c>
       <c r="X3" t="n">
-        <v>138.8399672000966</v>
+        <v>12.0193785809456</v>
       </c>
       <c r="Y3" t="n">
         <v>5.74307948984999</v>
       </c>
       <c r="Z3" t="n">
-        <v>127.6411056518555</v>
+        <v>0.8205170327044584</v>
       </c>
       <c r="AA3" t="n">
         <v>20.43361257999502</v>
       </c>
       <c r="AB3" t="n">
-        <v>95.12194775520489</v>
+        <v>-31.69864086394614</v>
       </c>
       <c r="AC3" t="n">
         <v>33.86397260300659</v>
       </c>
       <c r="AD3" t="n">
-        <v>68.98603236421627</v>
+        <v>-57.83455625493475</v>
       </c>
       <c r="AE3" t="n">
         <v>40.1068261329164</v>
@@ -987,6 +1083,42 @@
       </c>
       <c r="AX3" t="n">
         <v>1.302816291478969</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>1.184033838757775</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>2.257156870811072</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>2.257156870811072</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>0.744189297397156</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>4.595260268466603</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>-1.919390423097354</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>-1.919390423097354</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>0.1349798884886102</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>1.302816291478969</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>-0.7764976916210369</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>-0.7764976916210369</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>0.4439770688667639</v>
       </c>
     </row>
     <row r="4">
@@ -994,91 +1126,91 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>224.6799768285549</v>
+        <v>97.85938820940386</v>
       </c>
       <c r="C4" t="n">
         <v>7.388967148801122</v>
       </c>
       <c r="D4" t="n">
-        <v>209.99788375611</v>
+        <v>83.17729513695899</v>
       </c>
       <c r="E4" t="n">
         <v>17.97633069626828</v>
       </c>
       <c r="F4" t="n">
-        <v>190.7216792410993</v>
+        <v>63.90109062194824</v>
       </c>
       <c r="G4" t="n">
         <v>2.731485569730715</v>
       </c>
       <c r="H4" t="n">
-        <v>185.8178970661569</v>
+        <v>58.99730844700593</v>
       </c>
       <c r="I4" t="n">
         <v>4.475049769624754</v>
       </c>
       <c r="J4" t="n">
-        <v>186.0985045737409</v>
+        <v>59.27791595458987</v>
       </c>
       <c r="K4" t="n">
         <v>15.1720736889129</v>
       </c>
       <c r="L4" t="n">
-        <v>195.1675212129634</v>
+        <v>68.34693259381234</v>
       </c>
       <c r="M4" t="n">
         <v>18.89521416197432</v>
       </c>
       <c r="N4" t="n">
-        <v>191.3447511957047</v>
+        <v>64.52416257655364</v>
       </c>
       <c r="O4" t="n">
         <v>27.41107534854971</v>
       </c>
       <c r="P4" t="n">
-        <v>146.6015470788834</v>
+        <v>19.78095845973239</v>
       </c>
       <c r="Q4" t="n">
         <v>27.38348981167407</v>
       </c>
       <c r="R4" t="n">
-        <v>142.2808180464075</v>
+        <v>15.46022942725649</v>
       </c>
       <c r="S4" t="n">
         <v>20.23647795332239</v>
       </c>
       <c r="T4" t="n">
-        <v>150.9527997767672</v>
+        <v>24.13221115761616</v>
       </c>
       <c r="U4" t="n">
         <v>16.62493360803483</v>
       </c>
       <c r="V4" t="n">
-        <v>139.9264031268181</v>
+        <v>13.10581450766703</v>
       </c>
       <c r="W4" t="n">
         <v>11.81818779478682</v>
       </c>
       <c r="X4" t="n">
-        <v>149.2815423519053</v>
+        <v>22.46095373275431</v>
       </c>
       <c r="Y4" t="n">
         <v>5.583556154940993</v>
       </c>
       <c r="Z4" t="n">
-        <v>128.8802228075393</v>
+        <v>2.059634188388259</v>
       </c>
       <c r="AA4" t="n">
         <v>19.94621601510556</v>
       </c>
       <c r="AB4" t="n">
-        <v>97.5750984029567</v>
+        <v>-29.24549021619432</v>
       </c>
       <c r="AC4" t="n">
         <v>33.19516080491087</v>
       </c>
       <c r="AD4" t="n">
-        <v>98.97648425812419</v>
+        <v>-27.84410436102684</v>
       </c>
       <c r="AE4" t="n">
         <v>19.40288340791743</v>
@@ -1139,6 +1271,42 @@
       </c>
       <c r="AX4" t="n">
         <v>2.783323431284797</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>3.814358712309262</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>-1.472097521476405</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>-1.472097521476405</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>-1.802928234694223</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>2.484417180477804</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>-1.337780928307416</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>-1.337780928307416</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>-0.6080991563830656</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>2.783323431284797</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>0.877225742502</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>0.877225742502</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>-0.8766216297722524</v>
       </c>
     </row>
     <row r="5">
@@ -1146,91 +1314,91 @@
         <v>16</v>
       </c>
       <c r="B5" t="n">
-        <v>226.8158297589485</v>
+        <v>99.99524113979747</v>
       </c>
       <c r="C5" t="n">
         <v>7.605272658327792</v>
       </c>
       <c r="D5" t="n">
-        <v>212.3096750137654</v>
+        <v>85.48908639461436</v>
       </c>
       <c r="E5" t="n">
         <v>18.35517883300781</v>
       </c>
       <c r="F5" t="n">
-        <v>190.80618290191</v>
+        <v>63.98559428275899</v>
       </c>
       <c r="G5" t="n">
         <v>2.977898780335771</v>
       </c>
       <c r="H5" t="n">
-        <v>186.020103414008</v>
+        <v>59.19951479485697</v>
       </c>
       <c r="I5" t="n">
         <v>4.961963410073139</v>
       </c>
       <c r="J5" t="n">
-        <v>187.5228161507465</v>
+        <v>60.70222753159546</v>
       </c>
       <c r="K5" t="n">
         <v>15.69144877981633</v>
       </c>
       <c r="L5" t="n">
-        <v>196.7644539285214</v>
+        <v>69.94386530937035</v>
       </c>
       <c r="M5" t="n">
         <v>19.06887216770903</v>
       </c>
       <c r="N5" t="n">
-        <v>193.1038714469747</v>
+        <v>66.28328282782368</v>
       </c>
       <c r="O5" t="n">
         <v>27.65117604681787</v>
       </c>
       <c r="P5" t="n">
-        <v>149.9862752062209</v>
+        <v>23.16568658706991</v>
       </c>
       <c r="Q5" t="n">
         <v>27.314518867655</v>
       </c>
       <c r="R5" t="n">
-        <v>146.5647535121187</v>
+        <v>19.74416489296771</v>
       </c>
       <c r="S5" t="n">
         <v>19.04614631165848</v>
       </c>
       <c r="T5" t="n">
-        <v>155.9460599371727</v>
+        <v>29.12547131802173</v>
       </c>
       <c r="U5" t="n">
         <v>16.72768694289186</v>
       </c>
       <c r="V5" t="n">
-        <v>148.7886469414893</v>
+        <v>21.96805832233832</v>
       </c>
       <c r="W5" t="n">
         <v>7.123723943182753</v>
       </c>
       <c r="X5" t="n">
-        <v>159.5970174099537</v>
+        <v>32.77642879080264</v>
       </c>
       <c r="Y5" t="n">
         <v>4.9128065717981</v>
       </c>
       <c r="Z5" t="n">
-        <v>131.0225202682171</v>
+        <v>4.201931649066047</v>
       </c>
       <c r="AA5" t="n">
         <v>19.4160299098238</v>
       </c>
       <c r="AB5" t="n">
-        <v>99.30399630932099</v>
+        <v>-27.51659230983003</v>
       </c>
       <c r="AC5" t="n">
         <v>32.64216970890126</v>
       </c>
       <c r="AD5" t="n">
-        <v>72.40924023567365</v>
+        <v>-54.41134838347738</v>
       </c>
       <c r="AE5" t="n">
         <v>39.63574551521463</v>
@@ -1291,6 +1459,42 @@
       </c>
       <c r="AX5" t="n">
         <v>0.7573440520016144</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>-0.7670293529161452</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>-1.701537841783596</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>-1.701537841783596</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>1.286613246590038</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>-2.058822533043258</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>-1.756307955784955</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>-1.756307955784955</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>1.163634470504183</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>0.7573440520016144</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>-1.214621194836775</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>-1.214621194836775</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>0.2372103305528177</v>
       </c>
     </row>
     <row r="6">
@@ -1298,91 +1502,91 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>228.883578168585</v>
+        <v>102.062989549434</v>
       </c>
       <c r="C6" t="n">
         <v>7.352106621924868</v>
       </c>
       <c r="D6" t="n">
-        <v>214.4561032031445</v>
+        <v>87.63551458399346</v>
       </c>
       <c r="E6" t="n">
         <v>18.29470370678192</v>
       </c>
       <c r="F6" t="n">
-        <v>190.766485701216</v>
+        <v>63.94589708206502</v>
       </c>
       <c r="G6" t="n">
         <v>3.06276767811876</v>
       </c>
       <c r="H6" t="n">
-        <v>186.4678575637493</v>
+        <v>59.64726894459828</v>
       </c>
       <c r="I6" t="n">
         <v>5.434109302277264</v>
       </c>
       <c r="J6" t="n">
-        <v>188.7915246030118</v>
+        <v>61.97093598386077</v>
       </c>
       <c r="K6" t="n">
         <v>15.55400604897357</v>
       </c>
       <c r="L6" t="n">
-        <v>198.7235470021025</v>
+        <v>71.90295838295148</v>
       </c>
       <c r="M6" t="n">
         <v>19.18478620813249</v>
       </c>
       <c r="N6" t="n">
-        <v>194.9342514606232</v>
+        <v>68.11366284147219</v>
       </c>
       <c r="O6" t="n">
         <v>27.78302862289105</v>
       </c>
       <c r="P6" t="n">
-        <v>153.6711956592317</v>
+        <v>26.85060704008063</v>
       </c>
       <c r="Q6" t="n">
         <v>27.56054046306203</v>
       </c>
       <c r="R6" t="n">
-        <v>150.6568624618206</v>
+        <v>23.83627384266955</v>
       </c>
       <c r="S6" t="n">
         <v>18.85199851178108</v>
       </c>
       <c r="T6" t="n">
-        <v>160.003067584748</v>
+        <v>33.18247896559696</v>
       </c>
       <c r="U6" t="n">
         <v>16.60550705930019</v>
       </c>
       <c r="V6" t="n">
-        <v>155.2585561224755</v>
+        <v>28.43796750332444</v>
       </c>
       <c r="W6" t="n">
         <v>5.43458411034117</v>
       </c>
       <c r="X6" t="n">
-        <v>166.3407488072172</v>
+        <v>39.52016018806619</v>
       </c>
       <c r="Y6" t="n">
         <v>4.874939614153924</v>
       </c>
       <c r="Z6" t="n">
-        <v>133.6441567603578</v>
+        <v>6.823568141206799</v>
       </c>
       <c r="AA6" t="n">
         <v>18.95790100097656</v>
       </c>
       <c r="AB6" t="n">
-        <v>101.9638934033982</v>
+        <v>-24.85669521575279</v>
       </c>
       <c r="AC6" t="n">
         <v>32.37793902133373</v>
       </c>
       <c r="AD6" t="n">
-        <v>102.6433822956491</v>
+        <v>-24.17720632350191</v>
       </c>
       <c r="AE6" t="n">
         <v>19.43026400626974</v>
@@ -1443,6 +1647,42 @@
       </c>
       <c r="AX6" t="n">
         <v>-0.319794005070297</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>-0.2019644317813989</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>1.916074267086781</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>1.916074267086781</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>0.1199805735823192</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>-1.947524364547587</v>
+      </c>
+      <c r="BD6" t="n">
+        <v>1.352009253558509</v>
+      </c>
+      <c r="BE6" t="n">
+        <v>1.352009253558509</v>
+      </c>
+      <c r="BF6" t="n">
+        <v>0.2210796345178315</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>-0.319794005070297</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>-0.3053881382326495</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>-0.3053881382326495</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>0.4682041946471407</v>
       </c>
     </row>
     <row r="7">
@@ -1450,91 +1690,91 @@
         <v>24</v>
       </c>
       <c r="B7" t="n">
-        <v>231.0281021163819</v>
+        <v>104.2075134972309</v>
       </c>
       <c r="C7" t="n">
         <v>6.308636766798955</v>
       </c>
       <c r="D7" t="n">
-        <v>216.5102920633681</v>
+        <v>89.68970344421712</v>
       </c>
       <c r="E7" t="n">
         <v>17.5298569050241</v>
       </c>
       <c r="F7" t="n">
-        <v>190.5759375146095</v>
+        <v>63.75534889545846</v>
       </c>
       <c r="G7" t="n">
         <v>2.510464445073559</v>
       </c>
       <c r="H7" t="n">
-        <v>186.7088612089766</v>
+        <v>59.8882725898256</v>
       </c>
       <c r="I7" t="n">
         <v>5.04058269744224</v>
       </c>
       <c r="J7" t="n">
-        <v>190.858513243655</v>
+        <v>64.03792462450394</v>
       </c>
       <c r="K7" t="n">
         <v>15.19452764632854</v>
       </c>
       <c r="L7" t="n">
-        <v>200.5939397406071</v>
+        <v>73.7733511214561</v>
       </c>
       <c r="M7" t="n">
         <v>18.26575258944897</v>
       </c>
       <c r="N7" t="n">
-        <v>197.307898643169</v>
+        <v>70.48731002401797</v>
       </c>
       <c r="O7" t="n">
         <v>26.88343169841361</v>
       </c>
       <c r="P7" t="n">
-        <v>157.0367671073751</v>
+        <v>30.21617848822412</v>
       </c>
       <c r="Q7" t="n">
         <v>27.96672455807951</v>
       </c>
       <c r="R7" t="n">
-        <v>154.1754905213701</v>
+        <v>27.35490190221908</v>
       </c>
       <c r="S7" t="n">
         <v>19.07379475045712</v>
       </c>
       <c r="T7" t="n">
-        <v>164.0967267624875</v>
+        <v>37.27613814333652</v>
       </c>
       <c r="U7" t="n">
         <v>16.59030914306642</v>
       </c>
       <c r="V7" t="n">
-        <v>160.2651829415179</v>
+        <v>33.44459432236689</v>
       </c>
       <c r="W7" t="n">
         <v>4.863893224837938</v>
       </c>
       <c r="X7" t="n">
-        <v>172.0025742307623</v>
+        <v>45.18198561161121</v>
       </c>
       <c r="Y7" t="n">
         <v>4.339112626745354</v>
       </c>
       <c r="Z7" t="n">
-        <v>136.4223175860466</v>
+        <v>9.601728966895578</v>
       </c>
       <c r="AA7" t="n">
         <v>18.79712368579622</v>
       </c>
       <c r="AB7" t="n">
-        <v>104.4589144118289</v>
+        <v>-22.36167420732213</v>
       </c>
       <c r="AC7" t="n">
         <v>32.33782585631026</v>
       </c>
       <c r="AD7" t="n">
-        <v>77.73125831117024</v>
+        <v>-49.08933030798079</v>
       </c>
       <c r="AE7" t="n">
         <v>38.98217424433282</v>
@@ -1595,6 +1835,42 @@
       </c>
       <c r="AX7" t="n">
         <v>0.4758847164463544</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>0.8430227836826241</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>-1.399603072559327</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>-1.399603072559327</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>-0.8633603530540702</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>-0.9519076579805894</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>-0.2470974632117358</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>-0.2470974632117358</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>0.05271850376778675</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>0.4758847164463544</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>0.3151949718905231</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>0.3151949718905231</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>-0.4385780396946399</v>
       </c>
     </row>
     <row r="8">
@@ -1602,91 +1878,91 @@
         <v>28</v>
       </c>
       <c r="B8" t="n">
-        <v>233.1815670779411</v>
+        <v>106.3609784587901</v>
       </c>
       <c r="C8" t="n">
         <v>6.973181379602316</v>
       </c>
       <c r="D8" t="n">
-        <v>219.124258325455</v>
+        <v>92.30366970630402</v>
       </c>
       <c r="E8" t="n">
         <v>17.80756686596162</v>
       </c>
       <c r="F8" t="n">
-        <v>190.5253836449157</v>
+        <v>63.70479502576462</v>
       </c>
       <c r="G8" t="n">
         <v>2.979566695842351</v>
       </c>
       <c r="H8" t="n">
-        <v>188.3292411236053</v>
+        <v>61.5086525044543</v>
       </c>
       <c r="I8" t="n">
         <v>5.96490819403467</v>
       </c>
       <c r="J8" t="n">
-        <v>193.4529527704767</v>
+        <v>66.63236415132565</v>
       </c>
       <c r="K8" t="n">
         <v>15.769491804407</v>
       </c>
       <c r="L8" t="n">
-        <v>203.2137728751974</v>
+        <v>76.3931842560464</v>
       </c>
       <c r="M8" t="n">
         <v>18.88081976707947</v>
       </c>
       <c r="N8" t="n">
-        <v>199.930532942427</v>
+        <v>73.10994432327593</v>
       </c>
       <c r="O8" t="n">
         <v>27.4297409869255</v>
       </c>
       <c r="P8" t="n">
-        <v>159.5092996637872</v>
+        <v>32.68871104463619</v>
       </c>
       <c r="Q8" t="n">
         <v>27.46963095157705</v>
       </c>
       <c r="R8" t="n">
-        <v>157.3059893668966</v>
+        <v>30.48540074774559</v>
       </c>
       <c r="S8" t="n">
         <v>18.44722666638963</v>
       </c>
       <c r="T8" t="n">
-        <v>167.4407543020046</v>
+        <v>40.62016568285355</v>
       </c>
       <c r="U8" t="n">
         <v>15.96446747475483</v>
       </c>
       <c r="V8" t="n">
-        <v>163.9201012063534</v>
+        <v>37.09951258720234</v>
       </c>
       <c r="W8" t="n">
         <v>3.946868409501747</v>
       </c>
       <c r="X8" t="n">
-        <v>175.1651408824515</v>
+        <v>48.34455226330046</v>
       </c>
       <c r="Y8" t="n">
         <v>2.325691060816993</v>
       </c>
       <c r="Z8" t="n">
-        <v>139.1280153964428</v>
+        <v>12.30742677729182</v>
       </c>
       <c r="AA8" t="n">
         <v>18.30126985590509</v>
       </c>
       <c r="AB8" t="n">
-        <v>108.1325794788117</v>
+        <v>-18.6880091403393</v>
       </c>
       <c r="AC8" t="n">
         <v>32.31107224809363</v>
       </c>
       <c r="AD8" t="n">
-        <v>80.85557247730011</v>
+        <v>-45.9650161418509</v>
       </c>
       <c r="AE8" t="n">
         <v>39.6840440466049</v>
@@ -1747,6 +2023,42 @@
       </c>
       <c r="AX8" t="n">
         <v>-0.4827487208155539</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>-1.565431413069634</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>-0.4922453131727806</v>
+      </c>
+      <c r="BA8" t="n">
+        <v>-0.4922453131727806</v>
+      </c>
+      <c r="BB8" t="n">
+        <v>0.5458457241893566</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>0.254583063657555</v>
+      </c>
+      <c r="BD8" t="n">
+        <v>-0.06765936006563322</v>
+      </c>
+      <c r="BE8" t="n">
+        <v>-0.06765936006563322</v>
+      </c>
+      <c r="BF8" t="n">
+        <v>-0.9428062728206463</v>
+      </c>
+      <c r="BG8" t="n">
+        <v>-0.4827487208155539</v>
+      </c>
+      <c r="BH8" t="n">
+        <v>-0.5747002131881898</v>
+      </c>
+      <c r="BI8" t="n">
+        <v>-0.5747002131881898</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>-0.01744852505358829</v>
       </c>
     </row>
     <row r="9">
@@ -1754,91 +2066,91 @@
         <v>32</v>
       </c>
       <c r="B9" t="n">
-        <v>234.3688921091405</v>
+        <v>107.5483034899895</v>
       </c>
       <c r="C9" t="n">
         <v>6.626705413169034</v>
       </c>
       <c r="D9" t="n">
-        <v>221.9520727370648</v>
+        <v>95.13148411791376</v>
       </c>
       <c r="E9" t="n">
         <v>17.66260431167926</v>
       </c>
       <c r="F9" t="n">
-        <v>192.9931701497829</v>
+        <v>66.17258153063187</v>
       </c>
       <c r="G9" t="n">
         <v>3.556588355531076</v>
       </c>
       <c r="H9" t="n">
-        <v>193.0581731999174</v>
+        <v>66.23758458076642</v>
       </c>
       <c r="I9" t="n">
         <v>6.364911667844076</v>
       </c>
       <c r="J9" t="n">
-        <v>197.8758862678041</v>
+        <v>71.0552976486531</v>
       </c>
       <c r="K9" t="n">
         <v>15.94329184674201</v>
       </c>
       <c r="L9" t="n">
-        <v>206.9366683351233</v>
+        <v>80.11607971597226</v>
       </c>
       <c r="M9" t="n">
         <v>19.01311265661361</v>
       </c>
       <c r="N9" t="n">
-        <v>203.62485926202</v>
+        <v>76.804270642869</v>
       </c>
       <c r="O9" t="n">
         <v>27.3803690646557</v>
       </c>
       <c r="P9" t="n">
-        <v>161.3316089548964</v>
+        <v>34.51102033574532</v>
       </c>
       <c r="Q9" t="n">
         <v>27.27123017006732</v>
       </c>
       <c r="R9" t="n">
-        <v>158.916873120247</v>
+        <v>32.09628450109603</v>
       </c>
       <c r="S9" t="n">
         <v>18.37032399279006</v>
       </c>
       <c r="T9" t="n">
-        <v>168.4827449473929</v>
+        <v>41.66215632824188</v>
       </c>
       <c r="U9" t="n">
         <v>15.45216986473569</v>
       </c>
       <c r="V9" t="n">
-        <v>164.8881922376917</v>
+        <v>38.06760361854063</v>
       </c>
       <c r="W9" t="n">
         <v>3.702480234998326</v>
       </c>
       <c r="X9" t="n">
-        <v>176.3167675505293</v>
+        <v>49.4961789313783</v>
       </c>
       <c r="Y9" t="n">
         <v>1.680844895383139</v>
       </c>
       <c r="Z9" t="n">
-        <v>141.6930462451692</v>
+        <v>14.87245762601814</v>
       </c>
       <c r="AA9" t="n">
         <v>18.25281914244307</v>
       </c>
       <c r="AB9" t="n">
-        <v>110.4026429196622</v>
+        <v>-16.41794569948887</v>
       </c>
       <c r="AC9" t="n">
         <v>32.68563696678648</v>
       </c>
       <c r="AD9" t="n">
-        <v>82.81657442133479</v>
+        <v>-44.00401419781623</v>
       </c>
       <c r="AE9" t="n">
         <v>41.01299732289415</v>
@@ -1899,6 +2211,42 @@
       </c>
       <c r="AX9" t="n">
         <v>-1.511176258291815</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>-1.790502713064465</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>0.6777028347154874</v>
+      </c>
+      <c r="BA9" t="n">
+        <v>0.6777028347154874</v>
+      </c>
+      <c r="BB9" t="n">
+        <v>0.3964133578039825</v>
+      </c>
+      <c r="BC9" t="n">
+        <v>-2.310151305986886</v>
+      </c>
+      <c r="BD9" t="n">
+        <v>0.08256710719201399</v>
+      </c>
+      <c r="BE9" t="n">
+        <v>0.08256710719201399</v>
+      </c>
+      <c r="BF9" t="n">
+        <v>1.269031722178169</v>
+      </c>
+      <c r="BG9" t="n">
+        <v>-1.511176258291815</v>
+      </c>
+      <c r="BH9" t="n">
+        <v>0.1917357589288451</v>
+      </c>
+      <c r="BI9" t="n">
+        <v>0.1917357589288451</v>
+      </c>
+      <c r="BJ9" t="n">
+        <v>0.9663948597299845</v>
       </c>
     </row>
     <row r="10">
@@ -1906,91 +2254,91 @@
         <v>36</v>
       </c>
       <c r="B10" t="n">
-        <v>230.5560494039921</v>
+        <v>103.7354607848411</v>
       </c>
       <c r="C10" t="n">
         <v>11.09501047337309</v>
       </c>
       <c r="D10" t="n">
-        <v>224.9201963556574</v>
+        <v>98.09960773650636</v>
       </c>
       <c r="E10" t="n">
         <v>17.56929032346036</v>
       </c>
       <c r="F10" t="n">
-        <v>199.9948481295971</v>
+        <v>73.17425951044609</v>
       </c>
       <c r="G10" t="n">
         <v>4.14805310837766</v>
       </c>
       <c r="H10" t="n">
-        <v>200.0825795721501</v>
+        <v>73.26199095299906</v>
       </c>
       <c r="I10" t="n">
         <v>6.952878262134305</v>
       </c>
       <c r="J10" t="n">
-        <v>201.0767119996092</v>
+        <v>74.25612338045812</v>
       </c>
       <c r="K10" t="n">
         <v>16.95363876667428</v>
       </c>
       <c r="L10" t="n">
-        <v>210.4162832523915</v>
+        <v>83.59569463324043</v>
       </c>
       <c r="M10" t="n">
         <v>19.38868177698014</v>
       </c>
       <c r="N10" t="n">
-        <v>206.9126190023219</v>
+        <v>80.09203038317089</v>
       </c>
       <c r="O10" t="n">
         <v>27.54788094378532</v>
       </c>
       <c r="P10" t="n">
-        <v>163.7083276789239</v>
+        <v>36.8877390597729</v>
       </c>
       <c r="Q10" t="n">
         <v>26.67367813435008</v>
       </c>
       <c r="R10" t="n">
-        <v>160.4977851218366</v>
+        <v>33.67719650268555</v>
       </c>
       <c r="S10" t="n">
         <v>17.86993716625458</v>
       </c>
       <c r="T10" t="n">
-        <v>170.3057492032964</v>
+        <v>43.4851605841454</v>
       </c>
       <c r="U10" t="n">
         <v>14.8155577639316</v>
       </c>
       <c r="V10" t="n">
-        <v>165.3694416614289</v>
+        <v>38.54885304227786</v>
       </c>
       <c r="W10" t="n">
         <v>3.777719051279917</v>
       </c>
       <c r="X10" t="n">
-        <v>176.4617057556802</v>
+        <v>49.64111713652914</v>
       </c>
       <c r="Y10" t="n">
         <v>1.562995099006812</v>
       </c>
       <c r="Z10" t="n">
-        <v>144.4290343751299</v>
+        <v>17.60844575597888</v>
       </c>
       <c r="AA10" t="n">
         <v>18.76132234613947</v>
       </c>
       <c r="AB10" t="n">
-        <v>113.9668566115359</v>
+        <v>-12.85373200761511</v>
       </c>
       <c r="AC10" t="n">
         <v>32.34540046529568</v>
       </c>
       <c r="AD10" t="n">
-        <v>84.12568924274854</v>
+        <v>-42.6948993764025</v>
       </c>
       <c r="AE10" t="n">
         <v>40.65764001075258</v>
@@ -2051,6 +2399,42 @@
       </c>
       <c r="AX10" t="n">
         <v>1.325975643151861</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>-0.4299205818433669</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>-0.05167159723076242</v>
+      </c>
+      <c r="BA10" t="n">
+        <v>-0.05167159723076242</v>
+      </c>
+      <c r="BB10" t="n">
+        <v>-0.1435904966554278</v>
+      </c>
+      <c r="BC10" t="n">
+        <v>0.2012412130813503</v>
+      </c>
+      <c r="BD10" t="n">
+        <v>0.3855369880630115</v>
+      </c>
+      <c r="BE10" t="n">
+        <v>0.3855369880630115</v>
+      </c>
+      <c r="BF10" t="n">
+        <v>-0.7271065681724673</v>
+      </c>
+      <c r="BG10" t="n">
+        <v>1.325975643151861</v>
+      </c>
+      <c r="BH10" t="n">
+        <v>1.043393261416542</v>
+      </c>
+      <c r="BI10" t="n">
+        <v>1.043393261416542</v>
+      </c>
+      <c r="BJ10" t="n">
+        <v>-1.058569095719044</v>
       </c>
     </row>
     <row r="11">
@@ -2058,91 +2442,91 @@
         <v>40</v>
       </c>
       <c r="B11" t="n">
-        <v>195.0812684728745</v>
+        <v>68.26067985372343</v>
       </c>
       <c r="C11" t="n">
         <v>4.4564997896235</v>
       </c>
       <c r="D11" t="n">
-        <v>227.7276970604633</v>
+        <v>100.9071084413123</v>
       </c>
       <c r="E11" t="n">
         <v>17.63420510799327</v>
       </c>
       <c r="F11" t="n">
-        <v>205.3474147269066</v>
+        <v>78.52682610775562</v>
       </c>
       <c r="G11" t="n">
         <v>4.506322170825712</v>
       </c>
       <c r="H11" t="n">
-        <v>203.4780236000711</v>
+        <v>76.65743498092004</v>
       </c>
       <c r="I11" t="n">
         <v>7.758822339646365</v>
       </c>
       <c r="J11" t="n">
-        <v>203.2129891375278</v>
+        <v>76.3924005183768</v>
       </c>
       <c r="K11" t="n">
         <v>16.8825311863676</v>
       </c>
       <c r="L11" t="n">
-        <v>213.0701864019354</v>
+        <v>86.24959778278435</v>
       </c>
       <c r="M11" t="n">
         <v>19.39924118366647</v>
       </c>
       <c r="N11" t="n">
-        <v>209.8179588926599</v>
+        <v>82.99737027350889</v>
       </c>
       <c r="O11" t="n">
         <v>27.64287096388797</v>
       </c>
       <c r="P11" t="n">
-        <v>165.8987988816931</v>
+        <v>39.07821026254208</v>
       </c>
       <c r="Q11" t="n">
         <v>26.39448084729784</v>
       </c>
       <c r="R11" t="n">
-        <v>162.4629122145633</v>
+        <v>35.64232359541223</v>
       </c>
       <c r="S11" t="n">
         <v>17.76994339963223</v>
       </c>
       <c r="T11" t="n">
-        <v>172.2018820174197</v>
+        <v>45.38129339826867</v>
       </c>
       <c r="U11" t="n">
         <v>14.2499883124169</v>
       </c>
       <c r="V11" t="n">
-        <v>165.6112295515994</v>
+        <v>38.79064093244834</v>
       </c>
       <c r="W11" t="n">
         <v>3.967512414810514</v>
       </c>
       <c r="X11" t="n">
-        <v>176.5358305991964</v>
+        <v>49.71524198004539</v>
       </c>
       <c r="Y11" t="n">
         <v>1.563396859676288</v>
       </c>
       <c r="Z11" t="n">
-        <v>147.4679967190357</v>
+        <v>20.64740809988469</v>
       </c>
       <c r="AA11" t="n">
         <v>19.23830154094291</v>
       </c>
       <c r="AB11" t="n">
-        <v>116.9781116729087</v>
+        <v>-9.842476946242328</v>
       </c>
       <c r="AC11" t="n">
         <v>33.22361885233129</v>
       </c>
       <c r="AD11" t="n">
-        <v>85.96045717279962</v>
+        <v>-40.8601314463514</v>
       </c>
       <c r="AE11" t="n">
         <v>40.1313233882823</v>
@@ -2203,6 +2587,42 @@
       </c>
       <c r="AX11" t="n">
         <v>-0.07114883828063867</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>0.3562995627560204</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>0.8479355833300266</v>
+      </c>
+      <c r="BA11" t="n">
+        <v>0.8479355833300266</v>
+      </c>
+      <c r="BB11" t="n">
+        <v>-0.1670243775035262</v>
+      </c>
+      <c r="BC11" t="n">
+        <v>-0.1957925405402827</v>
+      </c>
+      <c r="BD11" t="n">
+        <v>0.3537053948043076</v>
+      </c>
+      <c r="BE11" t="n">
+        <v>0.3537053948043076</v>
+      </c>
+      <c r="BF11" t="n">
+        <v>0.7288778718079507</v>
+      </c>
+      <c r="BG11" t="n">
+        <v>-0.07114883828063867</v>
+      </c>
+      <c r="BH11" t="n">
+        <v>-1.126649731955526</v>
+      </c>
+      <c r="BI11" t="n">
+        <v>-1.126649731955526</v>
+      </c>
+      <c r="BJ11" t="n">
+        <v>0.6723280264736127</v>
       </c>
     </row>
     <row r="12">
@@ -2210,91 +2630,91 @@
         <v>44</v>
       </c>
       <c r="B12" t="n">
-        <v>217.8909854686007</v>
+        <v>91.07039684944968</v>
       </c>
       <c r="C12" t="n">
         <v>5.516470239517538</v>
       </c>
       <c r="D12" t="n">
-        <v>230.6392007685722</v>
+        <v>103.8186121494212</v>
       </c>
       <c r="E12" t="n">
         <v>17.19604248696185</v>
       </c>
       <c r="F12" t="n">
-        <v>211.1384314425448</v>
+        <v>84.31784282339382</v>
       </c>
       <c r="G12" t="n">
         <v>5.222401720412236</v>
       </c>
       <c r="H12" t="n">
-        <v>211.1250699834621</v>
+        <v>84.30448136431109</v>
       </c>
       <c r="I12" t="n">
         <v>8.347551873389705</v>
       </c>
       <c r="J12" t="n">
-        <v>207.7020401650287</v>
+        <v>80.88145154587767</v>
       </c>
       <c r="K12" t="n">
         <v>16.4364348066614</v>
       </c>
       <c r="L12" t="n">
-        <v>217.0588825611358</v>
+        <v>90.23829394198481</v>
       </c>
       <c r="M12" t="n">
         <v>19.07157492130361</v>
       </c>
       <c r="N12" t="n">
-        <v>213.6053790437414</v>
+        <v>86.7847904245904</v>
       </c>
       <c r="O12" t="n">
         <v>26.92367066728308</v>
       </c>
       <c r="P12" t="n">
-        <v>168.4533423565804</v>
+        <v>41.63275373742936</v>
       </c>
       <c r="Q12" t="n">
         <v>25.78543602152074</v>
       </c>
       <c r="R12" t="n">
-        <v>164.7650201269921</v>
+        <v>37.94443150784107</v>
       </c>
       <c r="S12" t="n">
         <v>17.12674485876206</v>
       </c>
       <c r="T12" t="n">
-        <v>174.2300601715737</v>
+        <v>47.40947155242272</v>
       </c>
       <c r="U12" t="n">
         <v>13.31957553295379</v>
       </c>
       <c r="V12" t="n">
-        <v>166.0056093905834</v>
+        <v>39.18502077143241</v>
       </c>
       <c r="W12" t="n">
         <v>3.853655875997347</v>
       </c>
       <c r="X12" t="n">
-        <v>176.4943863483186</v>
+        <v>49.67379772916753</v>
       </c>
       <c r="Y12" t="n">
         <v>1.096222248483215</v>
       </c>
       <c r="Z12" t="n">
-        <v>150.3688974583403</v>
+        <v>23.54830883918926</v>
       </c>
       <c r="AA12" t="n">
         <v>18.5469444761885</v>
       </c>
       <c r="AB12" t="n">
-        <v>121.1695691372486</v>
+        <v>-5.651019481902424</v>
       </c>
       <c r="AC12" t="n">
         <v>32.26548052848654</v>
       </c>
       <c r="AD12" t="n">
-        <v>88.67289766352229</v>
+        <v>-38.14769095562873</v>
       </c>
       <c r="AE12" t="n">
         <v>40.02956228053317</v>
@@ -2355,6 +2775,42 @@
       </c>
       <c r="AX12" t="n">
         <v>1.221038786181312</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>0.474422197341303</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>-0.132717565720645</v>
+      </c>
+      <c r="BA12" t="n">
+        <v>-0.132717565720645</v>
+      </c>
+      <c r="BB12" t="n">
+        <v>0.04263577673264818</v>
+      </c>
+      <c r="BC12" t="n">
+        <v>2.322685193069887</v>
+      </c>
+      <c r="BD12" t="n">
+        <v>0.8326010871659681</v>
+      </c>
+      <c r="BE12" t="n">
+        <v>0.8326010871659681</v>
+      </c>
+      <c r="BF12" t="n">
+        <v>-1.275890616695456</v>
+      </c>
+      <c r="BG12" t="n">
+        <v>1.221038786181312</v>
+      </c>
+      <c r="BH12" t="n">
+        <v>1.227949747465615</v>
+      </c>
+      <c r="BI12" t="n">
+        <v>1.227949747465615</v>
+      </c>
+      <c r="BJ12" t="n">
+        <v>-0.6976869913966774</v>
       </c>
     </row>
     <row r="13">
@@ -2362,91 +2818,91 @@
         <v>48</v>
       </c>
       <c r="B13" t="n">
-        <v>239.2112199296343</v>
+        <v>112.3906313104833</v>
       </c>
       <c r="C13" t="n">
         <v>7.372137840757972</v>
       </c>
       <c r="D13" t="n">
-        <v>233.2062454933816</v>
+        <v>106.3856568742306</v>
       </c>
       <c r="E13" t="n">
         <v>17.35498550090384</v>
       </c>
       <c r="F13" t="n">
-        <v>221.6796140404458</v>
+        <v>94.85902542129475</v>
       </c>
       <c r="G13" t="n">
         <v>5.630761004508805</v>
       </c>
       <c r="H13" t="n">
-        <v>220.554544824235</v>
+        <v>93.733956205084</v>
       </c>
       <c r="I13" t="n">
         <v>8.175752518024851</v>
       </c>
       <c r="J13" t="n">
-        <v>212.7714981424048</v>
+        <v>85.95090952325377</v>
       </c>
       <c r="K13" t="n">
         <v>15.94064590778756</v>
       </c>
       <c r="L13" t="n">
-        <v>221.0454508345178</v>
+        <v>94.22486221536678</v>
       </c>
       <c r="M13" t="n">
         <v>19.29408945935837</v>
       </c>
       <c r="N13" t="n">
-        <v>217.0727798279295</v>
+        <v>90.25219120877853</v>
       </c>
       <c r="O13" t="n">
         <v>26.66546436066323</v>
       </c>
       <c r="P13" t="n">
-        <v>170.4256372248873</v>
+        <v>43.60504860573627</v>
       </c>
       <c r="Q13" t="n">
         <v>25.57031956124814</v>
       </c>
       <c r="R13" t="n">
-        <v>166.2118333451292</v>
+        <v>39.39124472597811</v>
       </c>
       <c r="S13" t="n">
         <v>17.23808532065534</v>
       </c>
       <c r="T13" t="n">
-        <v>174.6565757913793</v>
+        <v>47.83598717222824</v>
       </c>
       <c r="U13" t="n">
         <v>12.1277910597781</v>
       </c>
       <c r="V13" t="n">
-        <v>166.0401800845532</v>
+        <v>39.21959146540213</v>
       </c>
       <c r="W13" t="n">
         <v>4.265233303638226</v>
       </c>
       <c r="X13" t="n">
-        <v>176.4695725542434</v>
+        <v>49.64898393509235</v>
       </c>
       <c r="Y13" t="n">
         <v>1.034850262581038</v>
       </c>
       <c r="Z13" t="n">
-        <v>152.4991116625198</v>
+        <v>25.67852304336875</v>
       </c>
       <c r="AA13" t="n">
         <v>19.44450621909284</v>
       </c>
       <c r="AB13" t="n">
-        <v>123.0967521667481</v>
+        <v>-3.723836452402963</v>
       </c>
       <c r="AC13" t="n">
         <v>33.55524184856009</v>
       </c>
       <c r="AD13" t="n">
-        <v>91.6604833399996</v>
+        <v>-35.16010527915142</v>
       </c>
       <c r="AE13" t="n">
         <v>41.65018771557099</v>
@@ -2507,6 +2963,42 @@
       </c>
       <c r="AX13" t="n">
         <v>-0.2775215549434469</v>
+      </c>
+      <c r="AY13" t="n">
+        <v>0.7630879388571783</v>
+      </c>
+      <c r="AZ13" t="n">
+        <v>-0.6362106956636098</v>
+      </c>
+      <c r="BA13" t="n">
+        <v>-0.6362106956636098</v>
+      </c>
+      <c r="BB13" t="n">
+        <v>-0.5053586456791567</v>
+      </c>
+      <c r="BC13" t="n">
+        <v>-0.2623995401017671</v>
+      </c>
+      <c r="BD13" t="n">
+        <v>-2.317277211950554</v>
+      </c>
+      <c r="BE13" t="n">
+        <v>-2.317277211950554</v>
+      </c>
+      <c r="BF13" t="n">
+        <v>0.2095049124340198</v>
+      </c>
+      <c r="BG13" t="n">
+        <v>-0.2775215549434469</v>
+      </c>
+      <c r="BH13" t="n">
+        <v>-1.060291633727309</v>
+      </c>
+      <c r="BI13" t="n">
+        <v>-1.060291633727309</v>
+      </c>
+      <c r="BJ13" t="n">
+        <v>0.4167350018014315</v>
       </c>
     </row>
     <row r="14">
@@ -2514,91 +3006,91 @@
         <v>52</v>
       </c>
       <c r="B14" t="n">
-        <v>241.9643646225016</v>
+        <v>115.1437760033506</v>
       </c>
       <c r="C14" t="n">
         <v>6.652081266362622</v>
       </c>
       <c r="D14" t="n">
-        <v>235.0072936808809</v>
+        <v>108.1867050617299</v>
       </c>
       <c r="E14" t="n">
         <v>17.03317926285115</v>
       </c>
       <c r="F14" t="n">
-        <v>226.1248658629174</v>
+        <v>99.30427724376638</v>
       </c>
       <c r="G14" t="n">
         <v>4.342294246592417</v>
       </c>
       <c r="H14" t="n">
-        <v>225.7391014631759</v>
+        <v>98.91851284402485</v>
       </c>
       <c r="I14" t="n">
         <v>7.229833399995833</v>
       </c>
       <c r="J14" t="n">
-        <v>215.3875208915549</v>
+        <v>88.56693227240382</v>
       </c>
       <c r="K14" t="n">
         <v>15.37655769510472</v>
       </c>
       <c r="L14" t="n">
-        <v>223.4565269439778</v>
+        <v>96.63593832482684</v>
       </c>
       <c r="M14" t="n">
         <v>18.79979397388215</v>
       </c>
       <c r="N14" t="n">
-        <v>219.2269543383983</v>
+        <v>92.40636571924735</v>
       </c>
       <c r="O14" t="n">
         <v>26.38467017640459</v>
       </c>
       <c r="P14" t="n">
-        <v>172.1986293792725</v>
+        <v>45.37804076012146</v>
       </c>
       <c r="Q14" t="n">
         <v>25.71343158153777</v>
       </c>
       <c r="R14" t="n">
-        <v>167.7553318916483</v>
+        <v>40.9347432724973</v>
       </c>
       <c r="S14" t="n">
         <v>17.59181732827043</v>
       </c>
       <c r="T14" t="n">
-        <v>175.3053198469446</v>
+        <v>48.4847312277936</v>
       </c>
       <c r="U14" t="n">
         <v>11.85706118319897</v>
       </c>
       <c r="V14" t="n">
-        <v>166.6505844035047</v>
+        <v>39.82999578435367</v>
       </c>
       <c r="W14" t="n">
         <v>5.152073312313</v>
       </c>
       <c r="X14" t="n">
-        <v>176.2295195396911</v>
+        <v>49.40893092054002</v>
       </c>
       <c r="Y14" t="n">
         <v>1.50930932227601</v>
       </c>
       <c r="Z14" t="n">
-        <v>155.0786809718355</v>
+        <v>28.25809235268452</v>
       </c>
       <c r="AA14" t="n">
         <v>20.27936894842918</v>
       </c>
       <c r="AB14" t="n">
-        <v>127.189735656089</v>
+        <v>0.3691470369379743</v>
       </c>
       <c r="AC14" t="n">
         <v>35.26130432778216</v>
       </c>
       <c r="AD14" t="n">
-        <v>95.29927436341632</v>
+        <v>-31.52131425573471</v>
       </c>
       <c r="AE14" t="n">
         <v>43.93882345645986</v>
@@ -2659,6 +3151,42 @@
       </c>
       <c r="AX14" t="n">
         <v>-0.1091418888624798</v>
+      </c>
+      <c r="AY14" t="n">
+        <v>-0.9696809023435731</v>
+      </c>
+      <c r="AZ14" t="n">
+        <v>0.1968620930324656</v>
+      </c>
+      <c r="BA14" t="n">
+        <v>0.1968620930324656</v>
+      </c>
+      <c r="BB14" t="n">
+        <v>0.70610464593814</v>
+      </c>
+      <c r="BC14" t="n">
+        <v>-2.009464623537342</v>
+      </c>
+      <c r="BD14" t="n">
+        <v>1.49923696084008</v>
+      </c>
+      <c r="BE14" t="n">
+        <v>1.49923696084008</v>
+      </c>
+      <c r="BF14" t="n">
+        <v>1.195623168519944</v>
+      </c>
+      <c r="BG14" t="n">
+        <v>-0.1091418888624798</v>
+      </c>
+      <c r="BH14" t="n">
+        <v>-0.2869088778396902</v>
+      </c>
+      <c r="BI14" t="n">
+        <v>-0.2869088778396902</v>
+      </c>
+      <c r="BJ14" t="n">
+        <v>-0.1857400490560686</v>
       </c>
     </row>
     <row r="15">
@@ -2666,91 +3194,91 @@
         <v>56</v>
       </c>
       <c r="B15" t="n">
-        <v>243.9975253920607</v>
+        <v>117.1769367729096</v>
       </c>
       <c r="C15" t="n">
         <v>7.18323322052651</v>
       </c>
       <c r="D15" t="n">
-        <v>236.4585742988485</v>
+        <v>109.6379856796975</v>
       </c>
       <c r="E15" t="n">
         <v>17.0958863927963</v>
       </c>
       <c r="F15" t="n">
-        <v>222.9494652849563</v>
+        <v>96.12887666580525</v>
       </c>
       <c r="G15" t="n">
         <v>5.000357932232795</v>
       </c>
       <c r="H15" t="n">
-        <v>228.8152105313667</v>
+        <v>101.9946219122156</v>
       </c>
       <c r="I15" t="n">
         <v>8.039778851448212</v>
       </c>
       <c r="J15" t="n">
-        <v>217.737471550069</v>
+        <v>90.91688293091798</v>
       </c>
       <c r="K15" t="n">
         <v>15.4686339358066</v>
       </c>
       <c r="L15" t="n">
-        <v>225.8470022932013</v>
+        <v>99.02641367405022</v>
       </c>
       <c r="M15" t="n">
         <v>18.737918772596</v>
       </c>
       <c r="N15" t="n">
-        <v>221.885849313533</v>
+        <v>95.065260694382</v>
       </c>
       <c r="O15" t="n">
         <v>26.49608774388089</v>
       </c>
       <c r="P15" t="n">
-        <v>174.0854121269064</v>
+        <v>47.26482350775538</v>
       </c>
       <c r="Q15" t="n">
         <v>25.41266299308614</v>
       </c>
       <c r="R15" t="n">
-        <v>169.712873215371</v>
+        <v>42.89228459621997</v>
       </c>
       <c r="S15" t="n">
         <v>17.34714102237783</v>
       </c>
       <c r="T15" t="n">
-        <v>176.6746236922893</v>
+        <v>49.8540350731383</v>
       </c>
       <c r="U15" t="n">
         <v>11.26709796012716</v>
       </c>
       <c r="V15" t="n">
-        <v>166.8893692341256</v>
+        <v>40.06878061497462</v>
       </c>
       <c r="W15" t="n">
         <v>6.177325958901264</v>
       </c>
       <c r="X15" t="n">
-        <v>176.2843061000743</v>
+        <v>49.46371748092326</v>
       </c>
       <c r="Y15" t="n">
         <v>1.602696357889378</v>
       </c>
       <c r="Z15" t="n">
-        <v>157.1397334971327</v>
+        <v>30.31914487798166</v>
       </c>
       <c r="AA15" t="n">
         <v>20.03433552194149</v>
       </c>
       <c r="AB15" t="n">
-        <v>130.218428753792</v>
+        <v>3.397840134640951</v>
       </c>
       <c r="AC15" t="n">
         <v>35.91243662732712</v>
       </c>
       <c r="AD15" t="n">
-        <v>99.33234275655546</v>
+        <v>-27.48824586259556</v>
       </c>
       <c r="AE15" t="n">
         <v>46.25929771585668</v>
@@ -2811,6 +3339,42 @@
       </c>
       <c r="AX15" t="n">
         <v>-0.6837224190057869</v>
+      </c>
+      <c r="AY15" t="n">
+        <v>0.1219688402082357</v>
+      </c>
+      <c r="AZ15" t="n">
+        <v>0.2585811841671515</v>
+      </c>
+      <c r="BA15" t="n">
+        <v>0.2585811841671515</v>
+      </c>
+      <c r="BB15" t="n">
+        <v>-0.1407100306609759</v>
+      </c>
+      <c r="BC15" t="n">
+        <v>1.025962967106858</v>
+      </c>
+      <c r="BD15" t="n">
+        <v>-0.8360084755579631</v>
+      </c>
+      <c r="BE15" t="n">
+        <v>-0.8360084755579631</v>
+      </c>
+      <c r="BF15" t="n">
+        <v>-1.176115419189416</v>
+      </c>
+      <c r="BG15" t="n">
+        <v>-0.6837224190057869</v>
+      </c>
+      <c r="BH15" t="n">
+        <v>0.2095033587413591</v>
+      </c>
+      <c r="BI15" t="n">
+        <v>0.2095033587413591</v>
+      </c>
+      <c r="BJ15" t="n">
+        <v>0.3300031735749271</v>
       </c>
     </row>
     <row r="16">
@@ -2818,91 +3382,91 @@
         <v>60</v>
       </c>
       <c r="B16" t="n">
-        <v>237.6895382049236</v>
+        <v>110.8689495857726</v>
       </c>
       <c r="C16" t="n">
         <v>6.590575360237288</v>
       </c>
       <c r="D16" t="n">
-        <v>237.7073482471578</v>
+        <v>110.8867596280068</v>
       </c>
       <c r="E16" t="n">
         <v>18.33412089246386</v>
       </c>
       <c r="F16" t="n">
-        <v>225.9415129397778</v>
+        <v>99.12092432062676</v>
       </c>
       <c r="G16" t="n">
         <v>5.703938260991528</v>
       </c>
       <c r="H16" t="n">
-        <v>223.0301042820545</v>
+        <v>96.20951566290351</v>
       </c>
       <c r="I16" t="n">
         <v>7.846621249584445</v>
       </c>
       <c r="J16" t="n">
-        <v>220.0263107076605</v>
+        <v>93.20572208850943</v>
       </c>
       <c r="K16" t="n">
         <v>15.67205875477893</v>
       </c>
       <c r="L16" t="n">
-        <v>228.3085786281748</v>
+        <v>101.4879900090238</v>
       </c>
       <c r="M16" t="n">
         <v>18.85922614564288</v>
       </c>
       <c r="N16" t="n">
-        <v>224.378695259703</v>
+        <v>97.55810664055193</v>
       </c>
       <c r="O16" t="n">
         <v>26.47283432331491</v>
       </c>
       <c r="P16" t="n">
-        <v>176.6489313003865</v>
+        <v>49.82834268123546</v>
       </c>
       <c r="Q16" t="n">
         <v>25.0290627175189</v>
       </c>
       <c r="R16" t="n">
-        <v>171.4389334333704</v>
+        <v>44.61834481421938</v>
       </c>
       <c r="S16" t="n">
         <v>17.46834694071018</v>
       </c>
       <c r="T16" t="n">
-        <v>177.5155879081564</v>
+        <v>50.69499928900538</v>
       </c>
       <c r="U16" t="n">
         <v>10.62595286267869</v>
       </c>
       <c r="V16" t="n">
-        <v>166.8659879806194</v>
+        <v>40.04539936146835</v>
       </c>
       <c r="W16" t="n">
         <v>7.21964734665891</v>
       </c>
       <c r="X16" t="n">
-        <v>176.0017364583117</v>
+        <v>49.18114783916067</v>
       </c>
       <c r="Y16" t="n">
         <v>1.707791267557347</v>
       </c>
       <c r="Z16" t="n">
-        <v>159.8827767879405</v>
+        <v>33.0621881687895</v>
       </c>
       <c r="AA16" t="n">
         <v>19.44492421251661</v>
       </c>
       <c r="AB16" t="n">
-        <v>132.7880534719914</v>
+        <v>5.967464852840351</v>
       </c>
       <c r="AC16" t="n">
         <v>34.91492981606341</v>
       </c>
       <c r="AD16" t="n">
-        <v>101.5326763721223</v>
+        <v>-25.28791224702876</v>
       </c>
       <c r="AE16" t="n">
         <v>44.26984178259018</v>
@@ -2963,6 +3527,42 @@
       </c>
       <c r="AX16" t="n">
         <v>0.06170974515061456</v>
+      </c>
+      <c r="AY16" t="n">
+        <v>0.650778460116141</v>
+      </c>
+      <c r="AZ16" t="n">
+        <v>-0.1251501885020709</v>
+      </c>
+      <c r="BA16" t="n">
+        <v>-0.1251501885020709</v>
+      </c>
+      <c r="BB16" t="n">
+        <v>-0.2658051889518074</v>
+      </c>
+      <c r="BC16" t="n">
+        <v>-0.6430711190066067</v>
+      </c>
+      <c r="BD16" t="n">
+        <v>0.796885338558234</v>
+      </c>
+      <c r="BE16" t="n">
+        <v>0.796885338558234</v>
+      </c>
+      <c r="BF16" t="n">
+        <v>0.7049876745748714</v>
+      </c>
+      <c r="BG16" t="n">
+        <v>0.06170974515061456</v>
+      </c>
+      <c r="BH16" t="n">
+        <v>1.256436966076226</v>
+      </c>
+      <c r="BI16" t="n">
+        <v>1.256436966076226</v>
+      </c>
+      <c r="BJ16" t="n">
+        <v>0.152621802606056</v>
       </c>
     </row>
     <row r="17">
@@ -2970,91 +3570,91 @@
         <v>64</v>
       </c>
       <c r="B17" t="n">
-        <v>226.0661901311672</v>
+        <v>99.24560151201617</v>
       </c>
       <c r="C17" t="n">
         <v>6.377110582716931</v>
       </c>
       <c r="D17" t="n">
-        <v>238.6905315550084</v>
+        <v>111.8699429358574</v>
       </c>
       <c r="E17" t="n">
         <v>19.84739100679438</v>
       </c>
       <c r="F17" t="n">
-        <v>228.1104062465911</v>
+        <v>101.2898176274401</v>
       </c>
       <c r="G17" t="n">
         <v>5.656433105468757</v>
       </c>
       <c r="H17" t="n">
-        <v>226.1972863623437</v>
+        <v>99.37669774319266</v>
       </c>
       <c r="I17" t="n">
         <v>8.082592740971997</v>
       </c>
       <c r="J17" t="n">
-        <v>222.8807814577793</v>
+        <v>96.06019283862825</v>
       </c>
       <c r="K17" t="n">
         <v>15.27660451036819</v>
       </c>
       <c r="L17" t="n">
-        <v>230.6323542239819</v>
+        <v>103.8117656048308</v>
       </c>
       <c r="M17" t="n">
         <v>18.49907408369349</v>
       </c>
       <c r="N17" t="n">
-        <v>226.705361173508</v>
+        <v>99.88477255435697</v>
       </c>
       <c r="O17" t="n">
         <v>26.23974820400807</v>
       </c>
       <c r="P17" t="n">
-        <v>178.3350974955457</v>
+        <v>51.51450887639473</v>
       </c>
       <c r="Q17" t="n">
         <v>24.83292843433137</v>
       </c>
       <c r="R17" t="n">
-        <v>173.1267330494333</v>
+        <v>46.30614443028228</v>
       </c>
       <c r="S17" t="n">
         <v>17.39215445011219</v>
       </c>
       <c r="T17" t="n">
-        <v>179.0047544114133</v>
+        <v>52.18416579226231</v>
       </c>
       <c r="U17" t="n">
         <v>10.35437482468625</v>
       </c>
       <c r="V17" t="n">
-        <v>167.5433158874511</v>
+        <v>40.72272726830014</v>
       </c>
       <c r="W17" t="n">
         <v>8.121892239185087</v>
       </c>
       <c r="X17" t="n">
-        <v>176.1333201793914</v>
+        <v>49.31273156024039</v>
       </c>
       <c r="Y17" t="n">
         <v>1.951306931515958</v>
       </c>
       <c r="Z17" t="n">
-        <v>162.3671450513475</v>
+        <v>35.54655643219645</v>
       </c>
       <c r="AA17" t="n">
         <v>18.3129980209026</v>
       </c>
       <c r="AB17" t="n">
-        <v>135.4630490566822</v>
+        <v>8.64246043753117</v>
       </c>
       <c r="AC17" t="n">
         <v>32.75091495919735</v>
       </c>
       <c r="AD17" t="n">
-        <v>103.7339149637425</v>
+        <v>-23.08667365540849</v>
       </c>
       <c r="AE17" t="n">
         <v>40.55855730746655</v>
@@ -3115,6 +3715,42 @@
       </c>
       <c r="AX17" t="n">
         <v>1.41762911973124</v>
+      </c>
+      <c r="AY17" t="n">
+        <v>0.1163673242168168</v>
+      </c>
+      <c r="AZ17" t="n">
+        <v>0.3221343487615593</v>
+      </c>
+      <c r="BA17" t="n">
+        <v>0.3221343487615593</v>
+      </c>
+      <c r="BB17" t="n">
+        <v>0.3274316336509344</v>
+      </c>
+      <c r="BC17" t="n">
+        <v>0.5078454931794143</v>
+      </c>
+      <c r="BD17" t="n">
+        <v>0.03809124902150685</v>
+      </c>
+      <c r="BE17" t="n">
+        <v>0.03809124902150685</v>
+      </c>
+      <c r="BF17" t="n">
+        <v>-0.1528595104157887</v>
+      </c>
+      <c r="BG17" t="n">
+        <v>1.41762911973124</v>
+      </c>
+      <c r="BH17" t="n">
+        <v>-1.304729204454603</v>
+      </c>
+      <c r="BI17" t="n">
+        <v>-1.304729204454603</v>
+      </c>
+      <c r="BJ17" t="n">
+        <v>-0.639648833934227</v>
       </c>
     </row>
     <row r="18">
@@ -3122,91 +3758,91 @@
         <v>68</v>
       </c>
       <c r="B18" t="n">
-        <v>230.153872405595</v>
+        <v>103.333283786444</v>
       </c>
       <c r="C18" t="n">
         <v>12.53670631571018</v>
       </c>
       <c r="D18" t="n">
-        <v>172.3372195629364</v>
+        <v>45.51663094378532</v>
       </c>
       <c r="E18" t="n">
         <v>23.33974635347408</v>
       </c>
       <c r="F18" t="n">
-        <v>230.4414538626975</v>
+        <v>103.6208652435465</v>
       </c>
       <c r="G18" t="n">
         <v>5.805283404411156</v>
       </c>
       <c r="H18" t="n">
-        <v>228.3070899070578</v>
+        <v>101.4865012879068</v>
       </c>
       <c r="I18" t="n">
         <v>7.826529157922621</v>
       </c>
       <c r="J18" t="n">
-        <v>225.0997278284519</v>
+        <v>98.27913920930092</v>
       </c>
       <c r="K18" t="n">
         <v>15.25784756274933</v>
       </c>
       <c r="L18" t="n">
-        <v>231.8608902553295</v>
+        <v>105.0403016361785</v>
       </c>
       <c r="M18" t="n">
         <v>18.41586904322848</v>
       </c>
       <c r="N18" t="n">
-        <v>228.1498187399925</v>
+        <v>101.3292301208415</v>
       </c>
       <c r="O18" t="n">
         <v>26.13224475941759</v>
       </c>
       <c r="P18" t="n">
-        <v>180.7916296289322</v>
+        <v>53.97104100978121</v>
       </c>
       <c r="Q18" t="n">
         <v>24.51602245898957</v>
       </c>
       <c r="R18" t="n">
-        <v>175.5626252356996</v>
+        <v>48.74203661654857</v>
       </c>
       <c r="S18" t="n">
         <v>16.96738790958486</v>
       </c>
       <c r="T18" t="n">
-        <v>180.3649212451692</v>
+        <v>53.54433262601813</v>
       </c>
       <c r="U18" t="n">
         <v>9.459089725575552</v>
       </c>
       <c r="V18" t="n">
-        <v>168.3836125312968</v>
+        <v>41.56302391214572</v>
       </c>
       <c r="W18" t="n">
         <v>9.252759243579618</v>
       </c>
       <c r="X18" t="n">
-        <v>175.9687565742655</v>
+        <v>49.14816795511447</v>
       </c>
       <c r="Y18" t="n">
         <v>1.983573588919135</v>
       </c>
       <c r="Z18" t="n">
-        <v>164.757468852591</v>
+        <v>37.93688023344001</v>
       </c>
       <c r="AA18" t="n">
         <v>17.63097073169465</v>
       </c>
       <c r="AB18" t="n">
-        <v>137.6588618501704</v>
+        <v>10.83827323101937</v>
       </c>
       <c r="AC18" t="n">
         <v>30.96539314757003</v>
       </c>
       <c r="AD18" t="n">
-        <v>107.4046845131732</v>
+        <v>-19.41590410597779</v>
       </c>
       <c r="AE18" t="n">
         <v>37.22360083397399</v>
@@ -3267,6 +3903,42 @@
       </c>
       <c r="AX18" t="n">
         <v>0.2149531585749571</v>
+      </c>
+      <c r="AY18" t="n">
+        <v>0.8916827229212303</v>
+      </c>
+      <c r="AZ18" t="n">
+        <v>0.1602218652250347</v>
+      </c>
+      <c r="BA18" t="n">
+        <v>0.1602218652250347</v>
+      </c>
+      <c r="BB18" t="n">
+        <v>-0.2075701688385772</v>
+      </c>
+      <c r="BC18" t="n">
+        <v>1.04732406370228</v>
+      </c>
+      <c r="BD18" t="n">
+        <v>-0.1120878346309897</v>
+      </c>
+      <c r="BE18" t="n">
+        <v>-0.1120878346309897</v>
+      </c>
+      <c r="BF18" t="n">
+        <v>-0.6003170636825019</v>
+      </c>
+      <c r="BG18" t="n">
+        <v>0.2149531585749571</v>
+      </c>
+      <c r="BH18" t="n">
+        <v>0.3098846283363792</v>
+      </c>
+      <c r="BI18" t="n">
+        <v>0.3098846283363792</v>
+      </c>
+      <c r="BJ18" t="n">
+        <v>-0.3595027138423588</v>
       </c>
     </row>
     <row r="19">
@@ -3274,91 +3946,91 @@
         <v>72</v>
       </c>
       <c r="B19" t="n">
-        <v>198.8716592179968</v>
+        <v>72.0510705988458</v>
       </c>
       <c r="C19" t="n">
         <v>14.02571049142391</v>
       </c>
       <c r="D19" t="n">
-        <v>207.0226554857924</v>
+        <v>80.20206686664133</v>
       </c>
       <c r="E19" t="n">
         <v>22.52036561357214</v>
       </c>
       <c r="F19" t="n">
-        <v>231.2902232433887</v>
+        <v>104.4696346242377</v>
       </c>
       <c r="G19" t="n">
         <v>5.891239896733715</v>
       </c>
       <c r="H19" t="n">
-        <v>225.9070081913725</v>
+        <v>99.0864195722215</v>
       </c>
       <c r="I19" t="n">
         <v>8.135718487678687</v>
       </c>
       <c r="J19" t="n">
-        <v>225.6077708081996</v>
+        <v>98.78718218904862</v>
       </c>
       <c r="K19" t="n">
         <v>15.42115312941531</v>
       </c>
       <c r="L19" t="n">
-        <v>233.0478085165329</v>
+        <v>106.2272198973818</v>
       </c>
       <c r="M19" t="n">
         <v>19.38382412524934</v>
       </c>
       <c r="N19" t="n">
-        <v>229.7716778643588</v>
+        <v>102.9510892452077</v>
       </c>
       <c r="O19" t="n">
         <v>26.48888648824489</v>
       </c>
       <c r="P19" t="n">
-        <v>182.5271109317212</v>
+        <v>55.70652231257014</v>
       </c>
       <c r="Q19" t="n">
         <v>24.69587123140376</v>
       </c>
       <c r="R19" t="n">
-        <v>177.7747387581684</v>
+        <v>50.95415013901732</v>
       </c>
       <c r="S19" t="n">
         <v>17.11786148395944</v>
       </c>
       <c r="T19" t="n">
-        <v>181.8426294529692</v>
+        <v>55.02204083381815</v>
       </c>
       <c r="U19" t="n">
         <v>9.142831031312333</v>
       </c>
       <c r="V19" t="n">
-        <v>169.3950267548256</v>
+        <v>42.57443813567463</v>
       </c>
       <c r="W19" t="n">
         <v>9.844573000644111</v>
       </c>
       <c r="X19" t="n">
-        <v>175.9838946322178</v>
+        <v>49.16330601306672</v>
       </c>
       <c r="Y19" t="n">
         <v>1.919036215924194</v>
       </c>
       <c r="Z19" t="n">
-        <v>166.5555203214605</v>
+        <v>39.73493170230948</v>
       </c>
       <c r="AA19" t="n">
         <v>17.33568881420378</v>
       </c>
       <c r="AB19" t="n">
-        <v>140.3328652077533</v>
+        <v>13.51227658860227</v>
       </c>
       <c r="AC19" t="n">
         <v>29.5603853590945</v>
       </c>
       <c r="AD19" t="n">
-        <v>109.1143445765719</v>
+        <v>-17.70624404257915</v>
       </c>
       <c r="AE19" t="n">
         <v>36.67406934372922</v>
@@ -3419,6 +4091,42 @@
       </c>
       <c r="AX19" t="n">
         <v>-2.425733657950761</v>
+      </c>
+      <c r="AY19" t="n">
+        <v>0.8367174462713352</v>
+      </c>
+      <c r="AZ19" t="n">
+        <v>-0.6063376801324081</v>
+      </c>
+      <c r="BA19" t="n">
+        <v>-0.6063376801324081</v>
+      </c>
+      <c r="BB19" t="n">
+        <v>-0.3818878044594626</v>
+      </c>
+      <c r="BC19" t="n">
+        <v>-0.814465620504861</v>
+      </c>
+      <c r="BD19" t="n">
+        <v>-0.4719443185595731</v>
+      </c>
+      <c r="BE19" t="n">
+        <v>-0.4719443185595731</v>
+      </c>
+      <c r="BF19" t="n">
+        <v>0.7923816366241688</v>
+      </c>
+      <c r="BG19" t="n">
+        <v>-2.425733657950761</v>
+      </c>
+      <c r="BH19" t="n">
+        <v>-0.7007346408027977</v>
+      </c>
+      <c r="BI19" t="n">
+        <v>-0.7007346408027977</v>
+      </c>
+      <c r="BJ19" t="n">
+        <v>1.577002903803111</v>
       </c>
     </row>
     <row r="20">
@@ -3426,91 +4134,91 @@
         <v>76</v>
       </c>
       <c r="B20" t="n">
-        <v>215.4697035379867</v>
+        <v>88.64911491883564</v>
       </c>
       <c r="C20" t="n">
         <v>20.25309826465363</v>
       </c>
       <c r="D20" t="n">
-        <v>225.371906145456</v>
+        <v>98.55131752630497</v>
       </c>
       <c r="E20" t="n">
         <v>20.31929949496655</v>
       </c>
       <c r="F20" t="n">
-        <v>231.8599224090576</v>
+        <v>105.0393337899066</v>
       </c>
       <c r="G20" t="n">
         <v>6.10938376568734</v>
       </c>
       <c r="H20" t="n">
-        <v>226.9666468843501</v>
+        <v>100.1460582651991</v>
       </c>
       <c r="I20" t="n">
         <v>8.545802501921962</v>
       </c>
       <c r="J20" t="n">
-        <v>227.4098216219151</v>
+        <v>100.5892330027641</v>
       </c>
       <c r="K20" t="n">
         <v>15.64816414041722</v>
       </c>
       <c r="L20" t="n">
-        <v>234.1213141350036</v>
+        <v>107.3007255158526</v>
       </c>
       <c r="M20" t="n">
         <v>19.4791225676841</v>
       </c>
       <c r="N20" t="n">
-        <v>230.9882302867605</v>
+        <v>104.1676416676095</v>
       </c>
       <c r="O20" t="n">
         <v>26.76935804651139</v>
       </c>
       <c r="P20" t="n">
-        <v>184.2162994628257</v>
+        <v>57.39571084367469</v>
       </c>
       <c r="Q20" t="n">
         <v>24.83383746857339</v>
       </c>
       <c r="R20" t="n">
-        <v>179.1408853327974</v>
+        <v>52.32029671364641</v>
       </c>
       <c r="S20" t="n">
         <v>17.41386575901763</v>
       </c>
       <c r="T20" t="n">
-        <v>183.1888949617427</v>
+        <v>56.36830634259164</v>
       </c>
       <c r="U20" t="n">
         <v>9.245462620511965</v>
       </c>
       <c r="V20" t="n">
-        <v>170.41658137707</v>
+        <v>43.59599275791896</v>
       </c>
       <c r="W20" t="n">
         <v>10.58007504077667</v>
       </c>
       <c r="X20" t="n">
-        <v>175.7071353019552</v>
+        <v>48.88654668280419</v>
       </c>
       <c r="Y20" t="n">
         <v>1.902324595349896</v>
       </c>
       <c r="Z20" t="n">
-        <v>168.1711146172057</v>
+        <v>41.35052599805469</v>
       </c>
       <c r="AA20" t="n">
         <v>17.85141559357338</v>
       </c>
       <c r="AB20" t="n">
-        <v>140.8644087771152</v>
+        <v>14.04382015796418</v>
       </c>
       <c r="AC20" t="n">
         <v>30.09501315177755</v>
       </c>
       <c r="AD20" t="n">
-        <v>109.6632105238894</v>
+        <v>-17.15737809526158</v>
       </c>
       <c r="AE20" t="n">
         <v>36.19005933721014</v>
@@ -3571,6 +4279,42 @@
       </c>
       <c r="AX20" t="n">
         <v>1.241591140735967</v>
+      </c>
+      <c r="AY20" t="n">
+        <v>-0.7457990482164103</v>
+      </c>
+      <c r="AZ20" t="n">
+        <v>-0.1263545291424484</v>
+      </c>
+      <c r="BA20" t="n">
+        <v>-0.1263545291424484</v>
+      </c>
+      <c r="BB20" t="n">
+        <v>0.6687275685202478</v>
+      </c>
+      <c r="BC20" t="n">
+        <v>0.4932712417846727</v>
+      </c>
+      <c r="BD20" t="n">
+        <v>0.3997171985847086</v>
+      </c>
+      <c r="BE20" t="n">
+        <v>0.3997171985847086</v>
+      </c>
+      <c r="BF20" t="n">
+        <v>-0.5251947537934185</v>
+      </c>
+      <c r="BG20" t="n">
+        <v>1.241591140735967</v>
+      </c>
+      <c r="BH20" t="n">
+        <v>1.100393351254233</v>
+      </c>
+      <c r="BI20" t="n">
+        <v>1.100393351254233</v>
+      </c>
+      <c r="BJ20" t="n">
+        <v>-1.491563240607305</v>
       </c>
     </row>
     <row r="21">
@@ -3578,91 +4322,91 @@
         <v>80</v>
       </c>
       <c r="B21" t="n">
-        <v>216.9931932015622</v>
+        <v>90.17260458241121</v>
       </c>
       <c r="C21" t="n">
         <v>21.93347443925573</v>
       </c>
       <c r="D21" t="n">
-        <v>193.9733038557337</v>
+        <v>67.15271523658265</v>
       </c>
       <c r="E21" t="n">
         <v>21.65144656566864</v>
       </c>
       <c r="F21" t="n">
-        <v>233.1161625841831</v>
+        <v>106.295573965032</v>
       </c>
       <c r="G21" t="n">
         <v>6.204706557253573</v>
       </c>
       <c r="H21" t="n">
-        <v>229.060665597307</v>
+        <v>102.2400769781559</v>
       </c>
       <c r="I21" t="n">
         <v>8.810643946870847</v>
       </c>
       <c r="J21" t="n">
-        <v>226.3226704394564</v>
+        <v>99.50208182030536</v>
       </c>
       <c r="K21" t="n">
         <v>16.77736322930519</v>
       </c>
       <c r="L21" t="n">
-        <v>235.7646668527989</v>
+        <v>108.9440782336479</v>
       </c>
       <c r="M21" t="n">
         <v>21.30740551238365</v>
       </c>
       <c r="N21" t="n">
-        <v>233.1218829180332</v>
+        <v>106.3012942988821</v>
       </c>
       <c r="O21" t="n">
         <v>27.67025967861744</v>
       </c>
       <c r="P21" t="n">
-        <v>186.4320237585839</v>
+        <v>59.61143513943287</v>
       </c>
       <c r="Q21" t="n">
         <v>25.18437973996426</v>
       </c>
       <c r="R21" t="n">
-        <v>181.2480652585943</v>
+        <v>54.42747663944326</v>
       </c>
       <c r="S21" t="n">
         <v>17.8044542353204</v>
       </c>
       <c r="T21" t="n">
-        <v>184.6952955773536</v>
+        <v>57.87470695820261</v>
       </c>
       <c r="U21" t="n">
         <v>9.266264895175368</v>
       </c>
       <c r="V21" t="n">
-        <v>171.4318884179947</v>
+        <v>44.61129979884368</v>
       </c>
       <c r="W21" t="n">
         <v>11.60619613972116</v>
       </c>
       <c r="X21" t="n">
-        <v>175.8928369968496</v>
+        <v>49.07224837769854</v>
       </c>
       <c r="Y21" t="n">
         <v>1.957313050615028</v>
       </c>
       <c r="Z21" t="n">
-        <v>169.9766493858176</v>
+        <v>43.15606076666652</v>
       </c>
       <c r="AA21" t="n">
         <v>18.068524624439</v>
       </c>
       <c r="AB21" t="n">
-        <v>142.1726165933812</v>
+        <v>15.35202797423018</v>
       </c>
       <c r="AC21" t="n">
         <v>30.59537360008727</v>
       </c>
       <c r="AD21" t="n">
-        <v>109.802091882584</v>
+        <v>-17.01849673656707</v>
       </c>
       <c r="AE21" t="n">
         <v>36.95487976074219</v>
@@ -3723,6 +4467,42 @@
       </c>
       <c r="AX21" t="n">
         <v>-1.057337023006526</v>
+      </c>
+      <c r="AY21" t="n">
+        <v>0.3465947313768356</v>
+      </c>
+      <c r="AZ21" t="n">
+        <v>0.4417156169444454</v>
+      </c>
+      <c r="BA21" t="n">
+        <v>0.4417156169444454</v>
+      </c>
+      <c r="BB21" t="n">
+        <v>-0.2177454518334778</v>
+      </c>
+      <c r="BC21" t="n">
+        <v>-0.2997709110994675</v>
+      </c>
+      <c r="BD21" t="n">
+        <v>-0.3450193890965103</v>
+      </c>
+      <c r="BE21" t="n">
+        <v>-0.3450193890965103</v>
+      </c>
+      <c r="BF21" t="n">
+        <v>0.2788612645340485</v>
+      </c>
+      <c r="BG21" t="n">
+        <v>-1.057337023006526</v>
+      </c>
+      <c r="BH21" t="n">
+        <v>-1.220784326871393</v>
+      </c>
+      <c r="BI21" t="n">
+        <v>-1.220784326871393</v>
+      </c>
+      <c r="BJ21" t="n">
+        <v>0.8133756134189249</v>
       </c>
     </row>
     <row r="22">
@@ -3730,91 +4510,91 @@
         <v>84</v>
       </c>
       <c r="B22" t="n">
-        <v>249.9608995749596</v>
+        <v>123.1403109558085</v>
       </c>
       <c r="C22" t="n">
         <v>21.1375540875374</v>
       </c>
       <c r="D22" t="n">
-        <v>178.9189338684082</v>
+        <v>52.09834524925718</v>
       </c>
       <c r="E22" t="n">
         <v>27.87714410335459</v>
       </c>
       <c r="F22" t="n">
-        <v>235.0636735875556</v>
+        <v>108.2430849684046</v>
       </c>
       <c r="G22" t="n">
         <v>5.813269919537476</v>
       </c>
       <c r="H22" t="n">
-        <v>232.4996585541583</v>
+        <v>105.6790699350073</v>
       </c>
       <c r="I22" t="n">
         <v>8.677332452002979</v>
       </c>
       <c r="J22" t="n">
-        <v>228.977740571854</v>
+        <v>102.157151952703</v>
       </c>
       <c r="K22" t="n">
         <v>17.04984624335106</v>
       </c>
       <c r="L22" t="n">
-        <v>237.0488264934814</v>
+        <v>110.2282378743304</v>
       </c>
       <c r="M22" t="n">
         <v>20.50053616787525</v>
       </c>
       <c r="N22" t="n">
-        <v>234.6195967907601</v>
+        <v>107.7990081716091</v>
       </c>
       <c r="O22" t="n">
         <v>27.75379546145175</v>
       </c>
       <c r="P22" t="n">
-        <v>188.1938366179771</v>
+        <v>61.37324799882607</v>
       </c>
       <c r="Q22" t="n">
         <v>25.40044987455327</v>
       </c>
       <c r="R22" t="n">
-        <v>182.9707500782419</v>
+        <v>56.15016145909086</v>
       </c>
       <c r="S22" t="n">
         <v>18.1092323140895</v>
       </c>
       <c r="T22" t="n">
-        <v>186.5629419367364</v>
+        <v>59.74235331758541</v>
       </c>
       <c r="U22" t="n">
         <v>9.470635272086923</v>
       </c>
       <c r="V22" t="n">
-        <v>172.4844729646723</v>
+        <v>45.66388434552129</v>
       </c>
       <c r="W22" t="n">
         <v>12.14971339448969</v>
       </c>
       <c r="X22" t="n">
-        <v>176.2277826349786</v>
+        <v>49.40719401582758</v>
       </c>
       <c r="Y22" t="n">
         <v>1.941112761801847</v>
       </c>
       <c r="Z22" t="n">
-        <v>171.7683102222199</v>
+        <v>44.94772160306892</v>
       </c>
       <c r="AA22" t="n">
         <v>18.46072014341962</v>
       </c>
       <c r="AB22" t="n">
-        <v>142.6068975570354</v>
+        <v>15.7863089378844</v>
       </c>
       <c r="AC22" t="n">
         <v>30.59562114959067</v>
       </c>
       <c r="AD22" t="n">
-        <v>110.4594433561285</v>
+        <v>-16.36114526302255</v>
       </c>
       <c r="AE22" t="n">
         <v>36.52777164540392</v>
@@ -3875,6 +4655,42 @@
       </c>
       <c r="AX22" t="n">
         <v>-0.1027627330733187</v>
+      </c>
+      <c r="AY22" t="n">
+        <v>0.5680067036361702</v>
+      </c>
+      <c r="AZ22" t="n">
+        <v>0.09990003723019814</v>
+      </c>
+      <c r="BA22" t="n">
+        <v>0.09990003723019814</v>
+      </c>
+      <c r="BB22" t="n">
+        <v>-0.05569736380043289</v>
+      </c>
+      <c r="BC22" t="n">
+        <v>0.0226319941525861</v>
+      </c>
+      <c r="BD22" t="n">
+        <v>0.6322817114663069</v>
+      </c>
+      <c r="BE22" t="n">
+        <v>0.6322817114663069</v>
+      </c>
+      <c r="BF22" t="n">
+        <v>-0.07388209296339643</v>
+      </c>
+      <c r="BG22" t="n">
+        <v>-0.1027627330733187</v>
+      </c>
+      <c r="BH22" t="n">
+        <v>1.779130854921191</v>
+      </c>
+      <c r="BI22" t="n">
+        <v>1.779130854921191</v>
+      </c>
+      <c r="BJ22" t="n">
+        <v>-0.04234236802604308</v>
       </c>
     </row>
     <row r="23">
@@ -3882,91 +4698,91 @@
         <v>88</v>
       </c>
       <c r="B23" t="n">
-        <v>187.8609434087226</v>
+        <v>61.04035478957157</v>
       </c>
       <c r="C23" t="n">
         <v>24.47585653751455</v>
       </c>
       <c r="D23" t="n">
-        <v>180.0387362216381</v>
+        <v>53.21814760248712</v>
       </c>
       <c r="E23" t="n">
         <v>28.06121745008104</v>
       </c>
       <c r="F23" t="n">
-        <v>215.9999441593251</v>
+        <v>89.17935554017411</v>
       </c>
       <c r="G23" t="n">
         <v>2.667394597479635</v>
       </c>
       <c r="H23" t="n">
-        <v>176.2660858478952</v>
+        <v>49.44549722874422</v>
       </c>
       <c r="I23" t="n">
         <v>22.63561005287983</v>
       </c>
       <c r="J23" t="n">
-        <v>214.9072971749814</v>
+        <v>88.08670855583031</v>
       </c>
       <c r="K23" t="n">
         <v>13.59430678347324</v>
       </c>
       <c r="L23" t="n">
-        <v>238.161357412947</v>
+        <v>111.340768793796</v>
       </c>
       <c r="M23" t="n">
         <v>20.5846461843937</v>
       </c>
       <c r="N23" t="n">
-        <v>235.735748486316</v>
+        <v>108.9151598671649</v>
       </c>
       <c r="O23" t="n">
         <v>27.92913152816449</v>
       </c>
       <c r="P23" t="n">
-        <v>190.2907777339854</v>
+        <v>63.4701891148344</v>
       </c>
       <c r="Q23" t="n">
         <v>25.93800159210855</v>
       </c>
       <c r="R23" t="n">
-        <v>184.6194977455951</v>
+        <v>57.79890912644407</v>
       </c>
       <c r="S23" t="n">
         <v>18.61362051456533</v>
       </c>
       <c r="T23" t="n">
-        <v>188.1505702404266</v>
+        <v>61.32998162127558</v>
       </c>
       <c r="U23" t="n">
         <v>10.36514931536734</v>
       </c>
       <c r="V23" t="n">
-        <v>174.6703513125155</v>
+        <v>47.84976269336453</v>
       </c>
       <c r="W23" t="n">
         <v>13.21938291509101</v>
       </c>
       <c r="X23" t="n">
-        <v>177.3629188537598</v>
+        <v>50.54233023460876</v>
       </c>
       <c r="Y23" t="n">
         <v>2.313382574852469</v>
       </c>
       <c r="Z23" t="n">
-        <v>173.4402879755548</v>
+        <v>46.61969935640379</v>
       </c>
       <c r="AA23" t="n">
         <v>18.88334396037649</v>
       </c>
       <c r="AB23" t="n">
-        <v>143.0591948488926</v>
+        <v>16.23860622974152</v>
       </c>
       <c r="AC23" t="n">
         <v>30.52975674892994</v>
       </c>
       <c r="AD23" t="n">
-        <v>111.1783088521755</v>
+        <v>-15.64227976697556</v>
       </c>
       <c r="AE23" t="n">
         <v>34.95622594305809</v>
@@ -4027,6 +4843,42 @@
       </c>
       <c r="AX23" t="n">
         <v>1.173253109288212</v>
+      </c>
+      <c r="AY23" t="n">
+        <v>0.7797305254835303</v>
+      </c>
+      <c r="AZ23" t="n">
+        <v>-0.1573516358399702</v>
+      </c>
+      <c r="BA23" t="n">
+        <v>-0.1573516358399702</v>
+      </c>
+      <c r="BB23" t="n">
+        <v>-0.1667443997165097</v>
+      </c>
+      <c r="BC23" t="n">
+        <v>0.7061687311585838</v>
+      </c>
+      <c r="BD23" t="n">
+        <v>-0.4912483796973774</v>
+      </c>
+      <c r="BE23" t="n">
+        <v>-0.4912483796973774</v>
+      </c>
+      <c r="BF23" t="n">
+        <v>-0.6356080579986062</v>
+      </c>
+      <c r="BG23" t="n">
+        <v>1.173253109288212</v>
+      </c>
+      <c r="BH23" t="n">
+        <v>-0.2077130053066267</v>
+      </c>
+      <c r="BI23" t="n">
+        <v>-0.2077130053066267</v>
+      </c>
+      <c r="BJ23" t="n">
+        <v>-0.5020115853115292</v>
       </c>
     </row>
     <row r="24">
@@ -4034,91 +4886,91 @@
         <v>92</v>
       </c>
       <c r="B24" t="n">
-        <v>189.7106637345984</v>
+        <v>62.89007511544737</v>
       </c>
       <c r="C24" t="n">
         <v>24.56342007251496</v>
       </c>
       <c r="D24" t="n">
-        <v>182.5317261066843</v>
+        <v>55.71113748753325</v>
       </c>
       <c r="E24" t="n">
         <v>28.03751357058261</v>
       </c>
       <c r="F24" t="n">
-        <v>215.9720867238146</v>
+        <v>89.1514981046636</v>
       </c>
       <c r="G24" t="n">
         <v>2.931298600866441</v>
       </c>
       <c r="H24" t="n">
-        <v>176.1797397694689</v>
+        <v>49.35915115031792</v>
       </c>
       <c r="I24" t="n">
         <v>22.52410726344332</v>
       </c>
       <c r="J24" t="n">
-        <v>215.90058752831</v>
+        <v>89.07999890915893</v>
       </c>
       <c r="K24" t="n">
         <v>13.93846552422706</v>
       </c>
       <c r="L24" t="n">
-        <v>176.0917582410447</v>
+        <v>49.27116962189373</v>
       </c>
       <c r="M24" t="n">
         <v>29.03276808718417</v>
       </c>
       <c r="N24" t="n">
-        <v>236.5885095076358</v>
+        <v>109.7679208884848</v>
       </c>
       <c r="O24" t="n">
         <v>28.29465663179437</v>
       </c>
       <c r="P24" t="n">
-        <v>192.4459071869546</v>
+        <v>65.62531856780356</v>
       </c>
       <c r="Q24" t="n">
         <v>26.26475882022939</v>
       </c>
       <c r="R24" t="n">
-        <v>186.8895348082198</v>
+        <v>60.06894618906873</v>
       </c>
       <c r="S24" t="n">
         <v>19.25463980816781</v>
       </c>
       <c r="T24" t="n">
-        <v>189.999539801415</v>
+        <v>63.17895118226398</v>
       </c>
       <c r="U24" t="n">
         <v>10.71746907335648</v>
       </c>
       <c r="V24" t="n">
-        <v>177.0921281043519</v>
+        <v>50.27153948520091</v>
       </c>
       <c r="W24" t="n">
         <v>13.98776034091382</v>
       </c>
       <c r="X24" t="n">
-        <v>178.2979559391103</v>
+        <v>51.47736731995928</v>
       </c>
       <c r="Y24" t="n">
         <v>2.823935163781996</v>
       </c>
       <c r="Z24" t="n">
-        <v>175.6820394637737</v>
+        <v>48.86145084462269</v>
       </c>
       <c r="AA24" t="n">
         <v>19.44476188497341</v>
       </c>
       <c r="AB24" t="n">
-        <v>144.9955351809238</v>
+        <v>18.17494656177277</v>
       </c>
       <c r="AC24" t="n">
         <v>30.978998224786</v>
       </c>
       <c r="AD24" t="n">
-        <v>111.9194720653778</v>
+        <v>-14.90111655377326</v>
       </c>
       <c r="AE24" t="n">
         <v>34.86377431991254</v>
@@ -4179,6 +5031,42 @@
       </c>
       <c r="AX24" t="n">
         <v>2.071085526627386</v>
+      </c>
+      <c r="AY24" t="n">
+        <v>0.5659446940882402</v>
+      </c>
+      <c r="AZ24" t="n">
+        <v>-0.05720862866066612</v>
+      </c>
+      <c r="BA24" t="n">
+        <v>-0.05720862866066612</v>
+      </c>
+      <c r="BB24" t="n">
+        <v>0.1654348520359248</v>
+      </c>
+      <c r="BC24" t="n">
+        <v>0.4968737454237084</v>
+      </c>
+      <c r="BD24" t="n">
+        <v>-0.4932897285084459</v>
+      </c>
+      <c r="BE24" t="n">
+        <v>-0.4932897285084459</v>
+      </c>
+      <c r="BF24" t="n">
+        <v>-0.305062102946999</v>
+      </c>
+      <c r="BG24" t="n">
+        <v>2.071085526627386</v>
+      </c>
+      <c r="BH24" t="n">
+        <v>-0.3655727995106957</v>
+      </c>
+      <c r="BI24" t="n">
+        <v>-0.3655727995106957</v>
+      </c>
+      <c r="BJ24" t="n">
+        <v>-1.240602262180038</v>
       </c>
     </row>
     <row r="25">
@@ -4186,91 +5074,91 @@
         <v>96</v>
       </c>
       <c r="B25" t="n">
-        <v>190.8750006493102</v>
+        <v>64.05441203015917</v>
       </c>
       <c r="C25" t="n">
         <v>24.12704305445894</v>
       </c>
       <c r="D25" t="n">
-        <v>183.8109158455057</v>
+        <v>56.99032722635471</v>
       </c>
       <c r="E25" t="n">
         <v>27.86596988109832</v>
       </c>
       <c r="F25" t="n">
-        <v>216.1387078305509</v>
+        <v>89.31811921139982</v>
       </c>
       <c r="G25" t="n">
         <v>2.477491662857375</v>
       </c>
       <c r="H25" t="n">
-        <v>239.2317759229782</v>
+        <v>112.4111873038272</v>
       </c>
       <c r="I25" t="n">
         <v>11.31926191614029</v>
       </c>
       <c r="J25" t="n">
-        <v>233.2077599586325</v>
+        <v>106.3871713394815</v>
       </c>
       <c r="K25" t="n">
         <v>16.34170045243931</v>
       </c>
       <c r="L25" t="n">
-        <v>217.731985132745</v>
+        <v>90.91139651359397</v>
       </c>
       <c r="M25" t="n">
         <v>18.8702603603931</v>
       </c>
       <c r="N25" t="n">
-        <v>237.1763903726923</v>
+        <v>110.3558017535412</v>
       </c>
       <c r="O25" t="n">
         <v>27.98539425464385</v>
       </c>
       <c r="P25" t="n">
-        <v>194.0560401754176</v>
+        <v>67.23545155626663</v>
       </c>
       <c r="Q25" t="n">
         <v>26.86990778496926</v>
       </c>
       <c r="R25" t="n">
-        <v>188.839948938248</v>
+        <v>62.01936031909699</v>
       </c>
       <c r="S25" t="n">
         <v>19.77052079870347</v>
       </c>
       <c r="T25" t="n">
-        <v>191.7498101579382</v>
+        <v>64.92922153878719</v>
       </c>
       <c r="U25" t="n">
         <v>11.08822924025516</v>
       </c>
       <c r="V25" t="n">
-        <v>178.7894796817861</v>
+        <v>51.96889106263504</v>
       </c>
       <c r="W25" t="n">
         <v>14.43820709877826</v>
       </c>
       <c r="X25" t="n">
-        <v>178.7890758920223</v>
+        <v>51.9684872728713</v>
       </c>
       <c r="Y25" t="n">
         <v>3.137109634724069</v>
       </c>
       <c r="Z25" t="n">
-        <v>177.0302569612544</v>
+        <v>50.20966834210336</v>
       </c>
       <c r="AA25" t="n">
         <v>19.91595004467256</v>
       </c>
       <c r="AB25" t="n">
-        <v>146.2064986533307</v>
+        <v>19.38591003417969</v>
       </c>
       <c r="AC25" t="n">
         <v>31.61976591069649</v>
       </c>
       <c r="AD25" t="n">
-        <v>112.6626197327959</v>
+        <v>-14.15796888635511</v>
       </c>
       <c r="AE25" t="n">
         <v>36.08174831309217</v>
@@ -4331,6 +5219,42 @@
       </c>
       <c r="AX25" t="n">
         <v>-0.3000211377479953</v>
+      </c>
+      <c r="AY25" t="n">
+        <v>0.781017735818768</v>
+      </c>
+      <c r="AZ25" t="n">
+        <v>0.04670781060286533</v>
+      </c>
+      <c r="BA25" t="n">
+        <v>0.04670781060286533</v>
+      </c>
+      <c r="BB25" t="n">
+        <v>-0.006337353266682388</v>
+      </c>
+      <c r="BC25" t="n">
+        <v>-0.4513505257625523</v>
+      </c>
+      <c r="BD25" t="n">
+        <v>-0.6353431301385113</v>
+      </c>
+      <c r="BE25" t="n">
+        <v>-0.6353431301385113</v>
+      </c>
+      <c r="BF25" t="n">
+        <v>0.5050855058792536</v>
+      </c>
+      <c r="BG25" t="n">
+        <v>-0.3000211377479953</v>
+      </c>
+      <c r="BH25" t="n">
+        <v>-1.079888431447917</v>
+      </c>
+      <c r="BI25" t="n">
+        <v>-1.079888431447917</v>
+      </c>
+      <c r="BJ25" t="n">
+        <v>1.020812686905545</v>
       </c>
     </row>
     <row r="26">
@@ -4338,91 +5262,91 @@
         <v>100</v>
       </c>
       <c r="B26" t="n">
-        <v>191.8389137755049</v>
+        <v>65.01832515635391</v>
       </c>
       <c r="C26" t="n">
         <v>23.49601907933013</v>
       </c>
       <c r="D26" t="n">
-        <v>184.2649865657725</v>
+        <v>57.44439794662149</v>
       </c>
       <c r="E26" t="n">
         <v>25.63061409808221</v>
       </c>
       <c r="F26" t="n">
-        <v>216.4201107430965</v>
+        <v>89.59952212394552</v>
       </c>
       <c r="G26" t="n">
         <v>2.107595890126333</v>
       </c>
       <c r="H26" t="n">
-        <v>178.1577455236557</v>
+        <v>51.33715690450467</v>
       </c>
       <c r="I26" t="n">
         <v>21.65722542620721</v>
       </c>
       <c r="J26" t="n">
-        <v>218.8748927826577</v>
+        <v>92.0543041635067</v>
       </c>
       <c r="K26" t="n">
         <v>13.64496109333444</v>
       </c>
       <c r="L26" t="n">
-        <v>219.0304208309093</v>
+        <v>92.20983221175825</v>
       </c>
       <c r="M26" t="n">
         <v>18.95230881711271</v>
       </c>
       <c r="N26" t="n">
-        <v>219.2477855276554</v>
+        <v>92.4271969085044</v>
       </c>
       <c r="O26" t="n">
         <v>27.21759714978808</v>
       </c>
       <c r="P26" t="n">
-        <v>195.866241860897</v>
+        <v>69.04565324174598</v>
       </c>
       <c r="Q26" t="n">
         <v>27.41486975487243</v>
       </c>
       <c r="R26" t="n">
-        <v>191.0688582887041</v>
+        <v>64.24826966955307</v>
       </c>
       <c r="S26" t="n">
         <v>20.16049648853058</v>
       </c>
       <c r="T26" t="n">
-        <v>194.0326690673828</v>
+        <v>67.21208044823182</v>
       </c>
       <c r="U26" t="n">
         <v>11.25618954922291</v>
       </c>
       <c r="V26" t="n">
-        <v>180.7934152319076</v>
+        <v>53.97282661275659</v>
       </c>
       <c r="W26" t="n">
         <v>14.72322991553774</v>
       </c>
       <c r="X26" t="n">
-        <v>179.5385786827574</v>
+        <v>52.71799006360642</v>
       </c>
       <c r="Y26" t="n">
         <v>3.742867327751</v>
       </c>
       <c r="Z26" t="n">
-        <v>178.7231242403071</v>
+        <v>51.9025356211561</v>
       </c>
       <c r="AA26" t="n">
         <v>20.21496549565742</v>
       </c>
       <c r="AB26" t="n">
-        <v>147.4512303129156</v>
+        <v>20.63064169376455</v>
       </c>
       <c r="AC26" t="n">
         <v>31.56995976224859</v>
       </c>
       <c r="AD26" t="n">
-        <v>113.9055657894054</v>
+        <v>-12.91502282974567</v>
       </c>
       <c r="AE26" t="n">
         <v>36.72155826649768</v>
@@ -4483,6 +5407,42 @@
       </c>
       <c r="AX26" t="n">
         <v>0.2191710949542625</v>
+      </c>
+      <c r="AY26" t="n">
+        <v>0.6661961754278494</v>
+      </c>
+      <c r="AZ26" t="n">
+        <v>-0.1148215603909186</v>
+      </c>
+      <c r="BA26" t="n">
+        <v>-0.1148215603909186</v>
+      </c>
+      <c r="BB26" t="n">
+        <v>-0.1615293709937839</v>
+      </c>
+      <c r="BC26" t="n">
+        <v>-0.3700951915560964</v>
+      </c>
+      <c r="BD26" t="n">
+        <v>0.08125533420645592</v>
+      </c>
+      <c r="BE26" t="n">
+        <v>0.08125533420645592</v>
+      </c>
+      <c r="BF26" t="n">
+        <v>0.7165984643449672</v>
+      </c>
+      <c r="BG26" t="n">
+        <v>0.2191710949542625</v>
+      </c>
+      <c r="BH26" t="n">
+        <v>0.5191922327022578</v>
+      </c>
+      <c r="BI26" t="n">
+        <v>0.5191922327022578</v>
+      </c>
+      <c r="BJ26" t="n">
+        <v>1.599080664150175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update DLC Approval true data since they had the bug in them ("Angle Velocity Velocity" etc.)
</commit_message>
<xml_diff>
--- a/tests/test_data/dlc_data/true_data/ID 12 - Run 3 - Average Stepcycle.xlsx
+++ b/tests/test_data/dlc_data/true_data/ID 12 - Run 3 - Average Stepcycle.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BJ26"/>
+  <dimension ref="A1:AX26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -591,69 +591,69 @@
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
+          <t>Hind paw tao Velocity</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Hind paw tao Acceleration</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Ankle Velocity</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Ankle Acceleration</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Knee Velocity</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Knee Acceleration</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Hip Velocity</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Hip Acceleration</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Iliac Crest Velocity</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Iliac Crest Acceleration</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
           <t>Ankle Angle</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Knee Angle</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Hip Angle</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>Hind paw tao Velocity</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>Hind paw tao Acceleration</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>Ankle Velocity</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>Ankle Acceleration</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>Knee Velocity</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>Knee Acceleration</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>Hip Velocity</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>Hip Acceleration</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>Iliac Crest Velocity</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>Iliac Crest Acceleration</t>
-        </is>
-      </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Ankle Angle Velocity</t>
@@ -682,66 +682,6 @@
       <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Hip Angle Acceleration</t>
-        </is>
-      </c>
-      <c r="AY1" s="1" t="inlineStr">
-        <is>
-          <t>Ankle Angle Velocity Velocity</t>
-        </is>
-      </c>
-      <c r="AZ1" s="1" t="inlineStr">
-        <is>
-          <t>Ankle Angle Velocity Acceleration</t>
-        </is>
-      </c>
-      <c r="BA1" s="1" t="inlineStr">
-        <is>
-          <t>Ankle Angle Acceleration Velocity</t>
-        </is>
-      </c>
-      <c r="BB1" s="1" t="inlineStr">
-        <is>
-          <t>Ankle Angle Acceleration Acceleration</t>
-        </is>
-      </c>
-      <c r="BC1" s="1" t="inlineStr">
-        <is>
-          <t>Knee Angle Velocity Velocity</t>
-        </is>
-      </c>
-      <c r="BD1" s="1" t="inlineStr">
-        <is>
-          <t>Knee Angle Velocity Acceleration</t>
-        </is>
-      </c>
-      <c r="BE1" s="1" t="inlineStr">
-        <is>
-          <t>Knee Angle Acceleration Velocity</t>
-        </is>
-      </c>
-      <c r="BF1" s="1" t="inlineStr">
-        <is>
-          <t>Knee Angle Acceleration Acceleration</t>
-        </is>
-      </c>
-      <c r="BG1" s="1" t="inlineStr">
-        <is>
-          <t>Hip Angle Velocity Velocity</t>
-        </is>
-      </c>
-      <c r="BH1" s="1" t="inlineStr">
-        <is>
-          <t>Hip Angle Velocity Acceleration</t>
-        </is>
-      </c>
-      <c r="BI1" s="1" t="inlineStr">
-        <is>
-          <t>Hip Angle Acceleration Velocity</t>
-        </is>
-      </c>
-      <c r="BJ1" s="1" t="inlineStr">
-        <is>
-          <t>Hip Angle Acceleration Acceleration</t>
         </is>
       </c>
     </row>
@@ -840,43 +780,43 @@
         <v>39.30151919101147</v>
       </c>
       <c r="AF2" t="n">
+        <v>4.684109383441022</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.04950229157794261</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>3.087160435128723</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>-0.6957302702234269</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>2.715521670402364</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.01782457879249399</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>1.098420772146671</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.1786526213300945</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.7469471464765931</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.2182894564689555</v>
+      </c>
+      <c r="AP2" t="n">
         <v>76.27841738596864</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AQ2" t="n">
         <v>41.78704621306755</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AR2" t="n">
         <v>108.938572679343</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>4.684109383441022</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0.04950229157794261</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>3.087160435128723</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>-0.6957302702234269</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>2.715521670402364</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0.01782457879249399</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>1.098420772146671</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0.1786526213300945</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.7469471464765931</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>0.2182894564689555</v>
       </c>
       <c r="AS2" t="n">
         <v>-6.564653501123261</v>
@@ -895,42 +835,6 @@
       </c>
       <c r="AX2" t="n">
         <v>1.598217427140197</v>
-      </c>
-      <c r="AY2" t="n">
-        <v>1.530466154794912</v>
-      </c>
-      <c r="AZ2" t="n">
-        <v>-1.773557206108463</v>
-      </c>
-      <c r="BA2" t="n">
-        <v>-1.773557206108463</v>
-      </c>
-      <c r="BB2" t="n">
-        <v>0.8686249019213583</v>
-      </c>
-      <c r="BC2" t="n">
-        <v>7.246022910409843</v>
-      </c>
-      <c r="BD2" t="n">
-        <v>0.3261180542288133</v>
-      </c>
-      <c r="BE2" t="n">
-        <v>0.3261180542288133</v>
-      </c>
-      <c r="BF2" t="n">
-        <v>-1.478764311488017</v>
-      </c>
-      <c r="BG2" t="n">
-        <v>1.598217427140197</v>
-      </c>
-      <c r="BH2" t="n">
-        <v>1.128723850572865</v>
-      </c>
-      <c r="BI2" t="n">
-        <v>1.128723850572865</v>
-      </c>
-      <c r="BJ2" t="n">
-        <v>-0.9391337800894628</v>
       </c>
     </row>
     <row r="3">
@@ -1028,43 +932,43 @@
         <v>40.1068261329164</v>
       </c>
       <c r="AF3" t="n">
+        <v>5.030683760947369</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0.1941488144245529</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>2.112853273432304</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0.1163797175630652</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>2.138412759659136</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>-0.2068697138035542</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>1.422397126542769</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0.1007531551604632</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>1.295953101300178</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>0.1935786389289937</v>
+      </c>
+      <c r="AP3" t="n">
         <v>64.36803110932706</v>
       </c>
-      <c r="AG3" t="n">
+      <c r="AQ3" t="n">
         <v>34.82074176464781</v>
       </c>
-      <c r="AH3" t="n">
+      <c r="AR3" t="n">
         <v>92.56358499492848</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>5.030683760947369</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>0.1941488144245529</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>2.112853273432304</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>0.1163797175630652</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>2.138412759659136</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>-0.2068697138035542</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>1.422397126542769</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>0.1007531551604632</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>1.295953101300178</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>0.1935786389289937</v>
       </c>
       <c r="AS3" t="n">
         <v>-6.913926847997542</v>
@@ -1083,42 +987,6 @@
       </c>
       <c r="AX3" t="n">
         <v>1.302816291478969</v>
-      </c>
-      <c r="AY3" t="n">
-        <v>1.184033838757775</v>
-      </c>
-      <c r="AZ3" t="n">
-        <v>2.257156870811072</v>
-      </c>
-      <c r="BA3" t="n">
-        <v>2.257156870811072</v>
-      </c>
-      <c r="BB3" t="n">
-        <v>0.744189297397156</v>
-      </c>
-      <c r="BC3" t="n">
-        <v>4.595260268466603</v>
-      </c>
-      <c r="BD3" t="n">
-        <v>-1.919390423097354</v>
-      </c>
-      <c r="BE3" t="n">
-        <v>-1.919390423097354</v>
-      </c>
-      <c r="BF3" t="n">
-        <v>0.1349798884886102</v>
-      </c>
-      <c r="BG3" t="n">
-        <v>1.302816291478969</v>
-      </c>
-      <c r="BH3" t="n">
-        <v>-0.7764976916210369</v>
-      </c>
-      <c r="BI3" t="n">
-        <v>-0.7764976916210369</v>
-      </c>
-      <c r="BJ3" t="n">
-        <v>0.4439770688667639</v>
       </c>
     </row>
     <row r="4">
@@ -1216,43 +1084,43 @@
         <v>19.40288340791743</v>
       </c>
       <c r="AF4" t="n">
+        <v>5.481331399146548</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>-0.03152502344009633</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>3.826746027520361</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0.8871240818754131</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>2.576745824610931</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>0.1591408506352803</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>1.971157560957241</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0.3050291791875228</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>1.637306619197769</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0.1354674075512197</v>
+      </c>
+      <c r="AP4" t="n">
         <v>57.19378018771658</v>
       </c>
-      <c r="AG4" t="n">
+      <c r="AQ4" t="n">
         <v>46.23547839009446</v>
       </c>
-      <c r="AH4" t="n">
+      <c r="AR4" t="n">
         <v>81.39986247642985</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>5.481331399146548</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>-0.03152502344009633</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>3.826746027520361</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>0.8871240818754131</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>2.576745824610931</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>0.1591408506352803</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>1.971157560957241</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>0.3050291791875228</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>1.637306619197769</v>
-      </c>
-      <c r="AR4" t="n">
-        <v>0.1354674075512197</v>
       </c>
       <c r="AS4" t="n">
         <v>1.765427288372468</v>
@@ -1271,42 +1139,6 @@
       </c>
       <c r="AX4" t="n">
         <v>2.783323431284797</v>
-      </c>
-      <c r="AY4" t="n">
-        <v>3.814358712309262</v>
-      </c>
-      <c r="AZ4" t="n">
-        <v>-1.472097521476405</v>
-      </c>
-      <c r="BA4" t="n">
-        <v>-1.472097521476405</v>
-      </c>
-      <c r="BB4" t="n">
-        <v>-1.802928234694223</v>
-      </c>
-      <c r="BC4" t="n">
-        <v>2.484417180477804</v>
-      </c>
-      <c r="BD4" t="n">
-        <v>-1.337780928307416</v>
-      </c>
-      <c r="BE4" t="n">
-        <v>-1.337780928307416</v>
-      </c>
-      <c r="BF4" t="n">
-        <v>-0.6080991563830656</v>
-      </c>
-      <c r="BG4" t="n">
-        <v>2.783323431284797</v>
-      </c>
-      <c r="BH4" t="n">
-        <v>0.877225742502</v>
-      </c>
-      <c r="BI4" t="n">
-        <v>0.877225742502</v>
-      </c>
-      <c r="BJ4" t="n">
-        <v>-0.8766216297722524</v>
       </c>
     </row>
     <row r="5">
@@ -1404,43 +1236,43 @@
         <v>39.63574551521463</v>
       </c>
       <c r="AF5" t="n">
+        <v>4.229330001993382</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>-0.892935915196194</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>4.109443502223236</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>-0.5980836584212916</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>2.173303035979576</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>-0.2340631282075858</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>2.067735347341983</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>-0.04795662900234454</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>1.683500979809047</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.0750480814183021</v>
+      </c>
+      <c r="AP5" t="n">
         <v>65.27696411534316</v>
       </c>
-      <c r="AG5" t="n">
+      <c r="AQ5" t="n">
         <v>67.58788373745234</v>
       </c>
-      <c r="AH5" t="n">
+      <c r="AR5" t="n">
         <v>81.3694336830704</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>4.229330001993382</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>-0.892935915196194</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>4.109443502223236</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>-0.5980836584212916</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>2.173303035979576</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>-0.2340631282075858</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>2.067735347341983</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>-0.04795662900234454</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>1.683500979809047</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>0.0750480814183021</v>
       </c>
       <c r="AS5" t="n">
         <v>4.556391338836856</v>
@@ -1459,42 +1291,6 @@
       </c>
       <c r="AX5" t="n">
         <v>0.7573440520016144</v>
-      </c>
-      <c r="AY5" t="n">
-        <v>-0.7670293529161452</v>
-      </c>
-      <c r="AZ5" t="n">
-        <v>-1.701537841783596</v>
-      </c>
-      <c r="BA5" t="n">
-        <v>-1.701537841783596</v>
-      </c>
-      <c r="BB5" t="n">
-        <v>1.286613246590038</v>
-      </c>
-      <c r="BC5" t="n">
-        <v>-2.058822533043258</v>
-      </c>
-      <c r="BD5" t="n">
-        <v>-1.756307955784955</v>
-      </c>
-      <c r="BE5" t="n">
-        <v>-1.756307955784955</v>
-      </c>
-      <c r="BF5" t="n">
-        <v>1.163634470504183</v>
-      </c>
-      <c r="BG5" t="n">
-        <v>0.7573440520016144</v>
-      </c>
-      <c r="BH5" t="n">
-        <v>-1.214621194836775</v>
-      </c>
-      <c r="BI5" t="n">
-        <v>-1.214621194836775</v>
-      </c>
-      <c r="BJ5" t="n">
-        <v>0.2372103305528177</v>
       </c>
     </row>
     <row r="6">
@@ -1592,43 +1388,43 @@
         <v>19.43026400626974</v>
       </c>
       <c r="AF6" t="n">
+        <v>2.932806725197651</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>-0.2704764934296335</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>2.590141905115004</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>-0.3658205904859191</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>2.097973417728504</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>0.009162882541085438</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>1.972124424386529</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>-0.143370222538076</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>1.806169875124667</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>-0.0798372512168104</v>
+      </c>
+      <c r="AP6" t="n">
         <v>70.29203063130515</v>
       </c>
-      <c r="AG6" t="n">
+      <c r="AQ6" t="n">
         <v>80.70499895263718</v>
       </c>
-      <c r="AH6" t="n">
+      <c r="AR6" t="n">
         <v>84.36838109771742</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>2.932806725197651</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>-0.2704764934296335</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>2.590141905115004</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>-0.3658205904859191</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>2.097973417728504</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>0.009162882541085438</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>1.972124424386529</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>-0.143370222538076</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>1.806169875124667</v>
-      </c>
-      <c r="AR6" t="n">
-        <v>-0.0798372512168104</v>
       </c>
       <c r="AS6" t="n">
         <v>0.5412040221668599</v>
@@ -1647,42 +1443,6 @@
       </c>
       <c r="AX6" t="n">
         <v>-0.319794005070297</v>
-      </c>
-      <c r="AY6" t="n">
-        <v>-0.2019644317813989</v>
-      </c>
-      <c r="AZ6" t="n">
-        <v>1.916074267086781</v>
-      </c>
-      <c r="BA6" t="n">
-        <v>1.916074267086781</v>
-      </c>
-      <c r="BB6" t="n">
-        <v>0.1199805735823192</v>
-      </c>
-      <c r="BC6" t="n">
-        <v>-1.947524364547587</v>
-      </c>
-      <c r="BD6" t="n">
-        <v>1.352009253558509</v>
-      </c>
-      <c r="BE6" t="n">
-        <v>1.352009253558509</v>
-      </c>
-      <c r="BF6" t="n">
-        <v>0.2210796345178315</v>
-      </c>
-      <c r="BG6" t="n">
-        <v>-0.319794005070297</v>
-      </c>
-      <c r="BH6" t="n">
-        <v>-0.3053881382326495</v>
-      </c>
-      <c r="BI6" t="n">
-        <v>-0.3053881382326495</v>
-      </c>
-      <c r="BJ6" t="n">
-        <v>0.4682041946471407</v>
       </c>
     </row>
     <row r="7">
@@ -1780,43 +1540,43 @@
         <v>38.98217424433282</v>
       </c>
       <c r="AF7" t="n">
+        <v>2.495509005607442</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>-0.6248146929639411</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>2.350000117687472</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>-0.3379271385517484</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>1.924529988714994</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>-0.1874079095556347</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>1.649854538288519</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>-0.09703230350575787</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>1.589057800617624</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>-0.2232597229328537</v>
+      </c>
+      <c r="AP7" t="n">
         <v>74.49923942014155</v>
       </c>
-      <c r="AG7" t="n">
+      <c r="AQ7" t="n">
         <v>86.03201670963168</v>
       </c>
-      <c r="AH7" t="n">
+      <c r="AR7" t="n">
         <v>86.08815249208324</v>
-      </c>
-      <c r="AI7" t="n">
-        <v>2.495509005607442</v>
-      </c>
-      <c r="AJ7" t="n">
-        <v>-0.6248146929639411</v>
-      </c>
-      <c r="AK7" t="n">
-        <v>2.350000117687472</v>
-      </c>
-      <c r="AL7" t="n">
-        <v>-0.3379271385517484</v>
-      </c>
-      <c r="AM7" t="n">
-        <v>1.924529988714994</v>
-      </c>
-      <c r="AN7" t="n">
-        <v>-0.1874079095556347</v>
-      </c>
-      <c r="AO7" t="n">
-        <v>1.649854538288519</v>
-      </c>
-      <c r="AP7" t="n">
-        <v>-0.09703230350575787</v>
-      </c>
-      <c r="AQ7" t="n">
-        <v>1.589057800617624</v>
-      </c>
-      <c r="AR7" t="n">
-        <v>-0.2232597229328537</v>
       </c>
       <c r="AS7" t="n">
         <v>4.190313773843986</v>
@@ -1835,42 +1595,6 @@
       </c>
       <c r="AX7" t="n">
         <v>0.4758847164463544</v>
-      </c>
-      <c r="AY7" t="n">
-        <v>0.8430227836826241</v>
-      </c>
-      <c r="AZ7" t="n">
-        <v>-1.399603072559327</v>
-      </c>
-      <c r="BA7" t="n">
-        <v>-1.399603072559327</v>
-      </c>
-      <c r="BB7" t="n">
-        <v>-0.8633603530540702</v>
-      </c>
-      <c r="BC7" t="n">
-        <v>-0.9519076579805894</v>
-      </c>
-      <c r="BD7" t="n">
-        <v>-0.2470974632117358</v>
-      </c>
-      <c r="BE7" t="n">
-        <v>-0.2470974632117358</v>
-      </c>
-      <c r="BF7" t="n">
-        <v>0.05271850376778675</v>
-      </c>
-      <c r="BG7" t="n">
-        <v>0.4758847164463544</v>
-      </c>
-      <c r="BH7" t="n">
-        <v>0.3151949718905231</v>
-      </c>
-      <c r="BI7" t="n">
-        <v>0.3151949718905231</v>
-      </c>
-      <c r="BJ7" t="n">
-        <v>-0.4385780396946399</v>
       </c>
     </row>
     <row r="8">
@@ -1968,43 +1692,43 @@
         <v>39.6840440466049</v>
       </c>
       <c r="AF8" t="n">
+        <v>0.836124825984875</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>-0.5027349959028555</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>1.030226971240754</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>-0.6717068083742905</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>0.9923128371543086</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>-0.5755092235321744</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>1.110723170828312</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>-0.3799037730440151</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>0.9267350460620669</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>-0.1625558163257335</v>
+      </c>
+      <c r="AP8" t="n">
         <v>82.07853934370844</v>
       </c>
-      <c r="AG8" t="n">
+      <c r="AQ8" t="n">
         <v>87.55140383470382</v>
       </c>
-      <c r="AH8" t="n">
+      <c r="AR8" t="n">
         <v>89.71146275223448</v>
-      </c>
-      <c r="AI8" t="n">
-        <v>0.836124825984875</v>
-      </c>
-      <c r="AJ8" t="n">
-        <v>-0.5027349959028555</v>
-      </c>
-      <c r="AK8" t="n">
-        <v>1.030226971240754</v>
-      </c>
-      <c r="AL8" t="n">
-        <v>-0.6717068083742905</v>
-      </c>
-      <c r="AM8" t="n">
-        <v>0.9923128371543086</v>
-      </c>
-      <c r="AN8" t="n">
-        <v>-0.5755092235321744</v>
-      </c>
-      <c r="AO8" t="n">
-        <v>1.110723170828312</v>
-      </c>
-      <c r="AP8" t="n">
-        <v>-0.3799037730440151</v>
-      </c>
-      <c r="AQ8" t="n">
-        <v>0.9267350460620669</v>
-      </c>
-      <c r="AR8" t="n">
-        <v>-0.1625558163257335</v>
       </c>
       <c r="AS8" t="n">
         <v>2.241011235283803</v>
@@ -2023,42 +1747,6 @@
       </c>
       <c r="AX8" t="n">
         <v>-0.4827487208155539</v>
-      </c>
-      <c r="AY8" t="n">
-        <v>-1.565431413069634</v>
-      </c>
-      <c r="AZ8" t="n">
-        <v>-0.4922453131727806</v>
-      </c>
-      <c r="BA8" t="n">
-        <v>-0.4922453131727806</v>
-      </c>
-      <c r="BB8" t="n">
-        <v>0.5458457241893566</v>
-      </c>
-      <c r="BC8" t="n">
-        <v>0.254583063657555</v>
-      </c>
-      <c r="BD8" t="n">
-        <v>-0.06765936006563322</v>
-      </c>
-      <c r="BE8" t="n">
-        <v>-0.06765936006563322</v>
-      </c>
-      <c r="BF8" t="n">
-        <v>-0.9428062728206463</v>
-      </c>
-      <c r="BG8" t="n">
-        <v>-0.4827487208155539</v>
-      </c>
-      <c r="BH8" t="n">
-        <v>-0.5747002131881898</v>
-      </c>
-      <c r="BI8" t="n">
-        <v>-0.5747002131881898</v>
-      </c>
-      <c r="BJ8" t="n">
-        <v>-0.01744852505358829</v>
       </c>
     </row>
     <row r="9">
@@ -2156,43 +1844,43 @@
         <v>41.01299732289415</v>
       </c>
       <c r="AF9" t="n">
+        <v>0.2731997916039006</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>-0.251672115731747</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>0.2892022437237642</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>-0.1217104019002644</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>0.6444880302916118</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>0.1952534026287971</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>0.8256313648629714</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>-0.007492937940231315</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>1.047614280213701</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>0.1386023582296119</v>
+      </c>
+      <c r="AP9" t="n">
         <v>83.39611361499679</v>
       </c>
-      <c r="AG9" t="n">
+      <c r="AQ9" t="n">
         <v>90.08912321440619</v>
       </c>
-      <c r="AH9" t="n">
+      <c r="AR9" t="n">
         <v>91.40377812912351</v>
-      </c>
-      <c r="AI9" t="n">
-        <v>0.2731997916039006</v>
-      </c>
-      <c r="AJ9" t="n">
-        <v>-0.251672115731747</v>
-      </c>
-      <c r="AK9" t="n">
-        <v>0.2892022437237642</v>
-      </c>
-      <c r="AL9" t="n">
-        <v>-0.1217104019002644</v>
-      </c>
-      <c r="AM9" t="n">
-        <v>0.6444880302916118</v>
-      </c>
-      <c r="AN9" t="n">
-        <v>0.1952534026287971</v>
-      </c>
-      <c r="AO9" t="n">
-        <v>0.8256313648629714</v>
-      </c>
-      <c r="AP9" t="n">
-        <v>-0.007492937940231315</v>
-      </c>
-      <c r="AQ9" t="n">
-        <v>1.047614280213701</v>
-      </c>
-      <c r="AR9" t="n">
-        <v>0.1386023582296119</v>
       </c>
       <c r="AS9" t="n">
         <v>-1.677272555967502</v>
@@ -2211,42 +1899,6 @@
       </c>
       <c r="AX9" t="n">
         <v>-1.511176258291815</v>
-      </c>
-      <c r="AY9" t="n">
-        <v>-1.790502713064465</v>
-      </c>
-      <c r="AZ9" t="n">
-        <v>0.6777028347154874</v>
-      </c>
-      <c r="BA9" t="n">
-        <v>0.6777028347154874</v>
-      </c>
-      <c r="BB9" t="n">
-        <v>0.3964133578039825</v>
-      </c>
-      <c r="BC9" t="n">
-        <v>-2.310151305986886</v>
-      </c>
-      <c r="BD9" t="n">
-        <v>0.08256710719201399</v>
-      </c>
-      <c r="BE9" t="n">
-        <v>0.08256710719201399</v>
-      </c>
-      <c r="BF9" t="n">
-        <v>1.269031722178169</v>
-      </c>
-      <c r="BG9" t="n">
-        <v>-1.511176258291815</v>
-      </c>
-      <c r="BH9" t="n">
-        <v>0.1917357589288451</v>
-      </c>
-      <c r="BI9" t="n">
-        <v>0.1917357589288451</v>
-      </c>
-      <c r="BJ9" t="n">
-        <v>0.9663948597299845</v>
       </c>
     </row>
     <row r="10">
@@ -2344,43 +1996,43 @@
         <v>40.65764001075258</v>
       </c>
       <c r="AF10" t="n">
+        <v>0.07499025223102507</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>-0.01770334040864796</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>0.2171171472427709</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>-0.05986538339168845</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>0.9289553824891428</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>0.01828213955493752</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>0.7635841978357227</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>0.09605377278429117</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>1.104298043758309</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>-0.04656188031460218</v>
+      </c>
+      <c r="AP10" t="n">
         <v>77.55167703402731</v>
       </c>
-      <c r="AG10" t="n">
+      <c r="AQ10" t="n">
         <v>83.38623737016098</v>
       </c>
-      <c r="AH10" t="n">
+      <c r="AR10" t="n">
         <v>87.05138847284528</v>
-      </c>
-      <c r="AI10" t="n">
-        <v>0.07499025223102507</v>
-      </c>
-      <c r="AJ10" t="n">
-        <v>-0.01770334040864796</v>
-      </c>
-      <c r="AK10" t="n">
-        <v>0.2171171472427709</v>
-      </c>
-      <c r="AL10" t="n">
-        <v>-0.05986538339168845</v>
-      </c>
-      <c r="AM10" t="n">
-        <v>0.9289553824891428</v>
-      </c>
-      <c r="AN10" t="n">
-        <v>0.01828213955493752</v>
-      </c>
-      <c r="AO10" t="n">
-        <v>0.7635841978357227</v>
-      </c>
-      <c r="AP10" t="n">
-        <v>0.09605377278429117</v>
-      </c>
-      <c r="AQ10" t="n">
-        <v>1.104298043758309</v>
-      </c>
-      <c r="AR10" t="n">
-        <v>-0.04656188031460218</v>
       </c>
       <c r="AS10" t="n">
         <v>-2.884745008356857</v>
@@ -2399,42 +2051,6 @@
       </c>
       <c r="AX10" t="n">
         <v>1.325975643151861</v>
-      </c>
-      <c r="AY10" t="n">
-        <v>-0.4299205818433669</v>
-      </c>
-      <c r="AZ10" t="n">
-        <v>-0.05167159723076242</v>
-      </c>
-      <c r="BA10" t="n">
-        <v>-0.05167159723076242</v>
-      </c>
-      <c r="BB10" t="n">
-        <v>-0.1435904966554278</v>
-      </c>
-      <c r="BC10" t="n">
-        <v>0.2012412130813503</v>
-      </c>
-      <c r="BD10" t="n">
-        <v>0.3855369880630115</v>
-      </c>
-      <c r="BE10" t="n">
-        <v>0.3855369880630115</v>
-      </c>
-      <c r="BF10" t="n">
-        <v>-0.7271065681724673</v>
-      </c>
-      <c r="BG10" t="n">
-        <v>1.325975643151861</v>
-      </c>
-      <c r="BH10" t="n">
-        <v>1.043393261416542</v>
-      </c>
-      <c r="BI10" t="n">
-        <v>1.043393261416542</v>
-      </c>
-      <c r="BJ10" t="n">
-        <v>-1.058569095719044</v>
       </c>
     </row>
     <row r="11">
@@ -2532,43 +2148,43 @@
         <v>40.1313233882823</v>
       </c>
       <c r="AF11" t="n">
+        <v>-0.02732733462718784</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>-0.02889227359852775</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>0.1237047479507787</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>0.03814798720339674</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>1.104405585755696</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>0.03301133500769282</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>1.253808305618609</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>0.08424520492554066</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>1.348180466509877</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>0.09101806802952694</v>
+      </c>
+      <c r="AP11" t="n">
         <v>69.98755812568433</v>
       </c>
-      <c r="AG11" t="n">
+      <c r="AQ11" t="n">
         <v>77.48831637824122</v>
       </c>
-      <c r="AH11" t="n">
+      <c r="AR11" t="n">
         <v>88.0029013891745</v>
-      </c>
-      <c r="AI11" t="n">
-        <v>-0.02732733462718784</v>
-      </c>
-      <c r="AJ11" t="n">
-        <v>-0.02889227359852775</v>
-      </c>
-      <c r="AK11" t="n">
-        <v>0.1237047479507787</v>
-      </c>
-      <c r="AL11" t="n">
-        <v>0.03814798720339674</v>
-      </c>
-      <c r="AM11" t="n">
-        <v>1.104405585755696</v>
-      </c>
-      <c r="AN11" t="n">
-        <v>0.03301133500769282</v>
-      </c>
-      <c r="AO11" t="n">
-        <v>1.253808305618609</v>
-      </c>
-      <c r="AP11" t="n">
-        <v>0.08424520492554066</v>
-      </c>
-      <c r="AQ11" t="n">
-        <v>1.348180466509877</v>
-      </c>
-      <c r="AR11" t="n">
-        <v>0.09101806802952694</v>
       </c>
       <c r="AS11" t="n">
         <v>-4.298903849669262</v>
@@ -2587,42 +2203,6 @@
       </c>
       <c r="AX11" t="n">
         <v>-0.07114883828063867</v>
-      </c>
-      <c r="AY11" t="n">
-        <v>0.3562995627560204</v>
-      </c>
-      <c r="AZ11" t="n">
-        <v>0.8479355833300266</v>
-      </c>
-      <c r="BA11" t="n">
-        <v>0.8479355833300266</v>
-      </c>
-      <c r="BB11" t="n">
-        <v>-0.1670243775035262</v>
-      </c>
-      <c r="BC11" t="n">
-        <v>-0.1957925405402827</v>
-      </c>
-      <c r="BD11" t="n">
-        <v>0.3537053948043076</v>
-      </c>
-      <c r="BE11" t="n">
-        <v>0.3537053948043076</v>
-      </c>
-      <c r="BF11" t="n">
-        <v>0.7288778718079507</v>
-      </c>
-      <c r="BG11" t="n">
-        <v>-0.07114883828063867</v>
-      </c>
-      <c r="BH11" t="n">
-        <v>-1.126649731955526</v>
-      </c>
-      <c r="BI11" t="n">
-        <v>-1.126649731955526</v>
-      </c>
-      <c r="BJ11" t="n">
-        <v>0.6723280264736127</v>
       </c>
     </row>
     <row r="12">
@@ -2720,43 +2300,43 @@
         <v>40.02956228053317</v>
       </c>
       <c r="AF12" t="n">
+        <v>0.03112529186492452</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>0.004157614200668291</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>0.1247137150865889</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>-0.08995228625358465</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>0.605603989134444</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>-0.4004156335871283</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>0.797397532361618</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>-0.2138236735729517</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>0.9808854853853255</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>-0.1455621516450929</v>
+      </c>
+      <c r="AP12" t="n">
         <v>63.84863746836543</v>
       </c>
-      <c r="AG12" t="n">
+      <c r="AQ12" t="n">
         <v>70.80722522416031</v>
       </c>
-      <c r="AH12" t="n">
+      <c r="AR12" t="n">
         <v>88.66981895238114</v>
-      </c>
-      <c r="AI12" t="n">
-        <v>0.03112529186492452</v>
-      </c>
-      <c r="AJ12" t="n">
-        <v>0.004157614200668291</v>
-      </c>
-      <c r="AK12" t="n">
-        <v>0.1247137150865889</v>
-      </c>
-      <c r="AL12" t="n">
-        <v>-0.08995228625358465</v>
-      </c>
-      <c r="AM12" t="n">
-        <v>0.605603989134444</v>
-      </c>
-      <c r="AN12" t="n">
-        <v>-0.4004156335871283</v>
-      </c>
-      <c r="AO12" t="n">
-        <v>0.797397532361618</v>
-      </c>
-      <c r="AP12" t="n">
-        <v>-0.2138236735729517</v>
-      </c>
-      <c r="AQ12" t="n">
-        <v>0.9808854853853255</v>
-      </c>
-      <c r="AR12" t="n">
-        <v>-0.1455621516450929</v>
       </c>
       <c r="AS12" t="n">
         <v>-2.321320357661561</v>
@@ -2775,42 +2355,6 @@
       </c>
       <c r="AX12" t="n">
         <v>1.221038786181312</v>
-      </c>
-      <c r="AY12" t="n">
-        <v>0.474422197341303</v>
-      </c>
-      <c r="AZ12" t="n">
-        <v>-0.132717565720645</v>
-      </c>
-      <c r="BA12" t="n">
-        <v>-0.132717565720645</v>
-      </c>
-      <c r="BB12" t="n">
-        <v>0.04263577673264818</v>
-      </c>
-      <c r="BC12" t="n">
-        <v>2.322685193069887</v>
-      </c>
-      <c r="BD12" t="n">
-        <v>0.8326010871659681</v>
-      </c>
-      <c r="BE12" t="n">
-        <v>0.8326010871659681</v>
-      </c>
-      <c r="BF12" t="n">
-        <v>-1.275890616695456</v>
-      </c>
-      <c r="BG12" t="n">
-        <v>1.221038786181312</v>
-      </c>
-      <c r="BH12" t="n">
-        <v>1.227949747465615</v>
-      </c>
-      <c r="BI12" t="n">
-        <v>1.227949747465615</v>
-      </c>
-      <c r="BJ12" t="n">
-        <v>-0.6976869913966774</v>
       </c>
     </row>
     <row r="13">
@@ -2908,43 +2452,43 @@
         <v>41.65018771557099</v>
       </c>
       <c r="AF13" t="n">
+        <v>-0.08278653976765327</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>-0.05380980511928612</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>0.1569747924804723</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>0.1439584062454529</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>0.170687918967392</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>0.0555571089399578</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>0.7858753204345703</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>0.02417133209553768</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>1.01107130659388</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>-0.04982567848043118</v>
+      </c>
+      <c r="AP13" t="n">
         <v>59.60740560041176</v>
       </c>
-      <c r="AG13" t="n">
+      <c r="AQ13" t="n">
         <v>73.41687484235894</v>
       </c>
-      <c r="AH13" t="n">
+      <c r="AR13" t="n">
         <v>94.22089166031304</v>
-      </c>
-      <c r="AI13" t="n">
-        <v>-0.08278653976765327</v>
-      </c>
-      <c r="AJ13" t="n">
-        <v>-0.05380980511928612</v>
-      </c>
-      <c r="AK13" t="n">
-        <v>0.1569747924804723</v>
-      </c>
-      <c r="AL13" t="n">
-        <v>0.1439584062454529</v>
-      </c>
-      <c r="AM13" t="n">
-        <v>0.170687918967392</v>
-      </c>
-      <c r="AN13" t="n">
-        <v>0.0555571089399578</v>
-      </c>
-      <c r="AO13" t="n">
-        <v>0.7858753204345703</v>
-      </c>
-      <c r="AP13" t="n">
-        <v>0.02417133209553768</v>
-      </c>
-      <c r="AQ13" t="n">
-        <v>1.01107130659388</v>
-      </c>
-      <c r="AR13" t="n">
-        <v>-0.04982567848043118</v>
       </c>
       <c r="AS13" t="n">
         <v>-0.8746071285364394</v>
@@ -2963,42 +2507,6 @@
       </c>
       <c r="AX13" t="n">
         <v>-0.2775215549434469</v>
-      </c>
-      <c r="AY13" t="n">
-        <v>0.7630879388571783</v>
-      </c>
-      <c r="AZ13" t="n">
-        <v>-0.6362106956636098</v>
-      </c>
-      <c r="BA13" t="n">
-        <v>-0.6362106956636098</v>
-      </c>
-      <c r="BB13" t="n">
-        <v>-0.5053586456791567</v>
-      </c>
-      <c r="BC13" t="n">
-        <v>-0.2623995401017671</v>
-      </c>
-      <c r="BD13" t="n">
-        <v>-2.317277211950554</v>
-      </c>
-      <c r="BE13" t="n">
-        <v>-2.317277211950554</v>
-      </c>
-      <c r="BF13" t="n">
-        <v>0.2095049124340198</v>
-      </c>
-      <c r="BG13" t="n">
-        <v>-0.2775215549434469</v>
-      </c>
-      <c r="BH13" t="n">
-        <v>-1.060291633727309</v>
-      </c>
-      <c r="BI13" t="n">
-        <v>-1.060291633727309</v>
-      </c>
-      <c r="BJ13" t="n">
-        <v>0.4167350018014315</v>
       </c>
     </row>
     <row r="14">
@@ -3096,43 +2604,43 @@
         <v>43.93882345645986</v>
       </c>
       <c r="AF14" t="n">
+        <v>-0.09969853340310664</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>0.07370989373389492</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>0.1891734752249157</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>-0.09290487208264686</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>0.4923003785153632</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>0.1801399474448342</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>0.8802129867229027</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>0.1035106943008692</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>0.7668819833309115</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>0.02844764831218427</v>
+      </c>
+      <c r="AP14" t="n">
         <v>58.4185254878868</v>
       </c>
-      <c r="AG14" t="n">
+      <c r="AQ14" t="n">
         <v>74.9769263001505</v>
       </c>
-      <c r="AH14" t="n">
+      <c r="AR14" t="n">
         <v>98.66187814847117</v>
-      </c>
-      <c r="AI14" t="n">
-        <v>-0.09969853340310664</v>
-      </c>
-      <c r="AJ14" t="n">
-        <v>0.07370989373389492</v>
-      </c>
-      <c r="AK14" t="n">
-        <v>0.1891734752249157</v>
-      </c>
-      <c r="AL14" t="n">
-        <v>-0.09290487208264686</v>
-      </c>
-      <c r="AM14" t="n">
-        <v>0.4923003785153632</v>
-      </c>
-      <c r="AN14" t="n">
-        <v>0.1801399474448342</v>
-      </c>
-      <c r="AO14" t="n">
-        <v>0.8802129867229027</v>
-      </c>
-      <c r="AP14" t="n">
-        <v>0.1035106943008692</v>
-      </c>
-      <c r="AQ14" t="n">
-        <v>0.7668819833309115</v>
-      </c>
-      <c r="AR14" t="n">
-        <v>0.02844764831218427</v>
       </c>
       <c r="AS14" t="n">
         <v>-1.972736682065757</v>
@@ -3151,42 +2659,6 @@
       </c>
       <c r="AX14" t="n">
         <v>-0.1091418888624798</v>
-      </c>
-      <c r="AY14" t="n">
-        <v>-0.9696809023435731</v>
-      </c>
-      <c r="AZ14" t="n">
-        <v>0.1968620930324656</v>
-      </c>
-      <c r="BA14" t="n">
-        <v>0.1968620930324656</v>
-      </c>
-      <c r="BB14" t="n">
-        <v>0.70610464593814</v>
-      </c>
-      <c r="BC14" t="n">
-        <v>-2.009464623537342</v>
-      </c>
-      <c r="BD14" t="n">
-        <v>1.49923696084008</v>
-      </c>
-      <c r="BE14" t="n">
-        <v>1.49923696084008</v>
-      </c>
-      <c r="BF14" t="n">
-        <v>1.195623168519944</v>
-      </c>
-      <c r="BG14" t="n">
-        <v>-0.1091418888624798</v>
-      </c>
-      <c r="BH14" t="n">
-        <v>-0.2869088778396902</v>
-      </c>
-      <c r="BI14" t="n">
-        <v>-0.2869088778396902</v>
-      </c>
-      <c r="BJ14" t="n">
-        <v>-0.1857400490560686</v>
       </c>
     </row>
     <row r="15">
@@ -3284,43 +2756,43 @@
         <v>46.25929771585668</v>
       </c>
       <c r="AF15" t="n">
+        <v>-0.02500351439131876</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>-0.08433905053646207</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>0.1330071307243195</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>-0.06554152103180577</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>0.6204564520653264</v>
+      </c>
+      <c r="AK15" t="n">
+        <v>-0.1320849073694035</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>1.021371496484637</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>-0.05787027643081366</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>1.374983280263045</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>0.1691841064615396</v>
+      </c>
+      <c r="AP15" t="n">
         <v>53.35092176598754</v>
       </c>
-      <c r="AG15" t="n">
+      <c r="AQ15" t="n">
         <v>68.49911926379269</v>
       </c>
-      <c r="AH15" t="n">
+      <c r="AR15" t="n">
         <v>102.6662970811794</v>
-      </c>
-      <c r="AI15" t="n">
-        <v>-0.02500351439131876</v>
-      </c>
-      <c r="AJ15" t="n">
-        <v>-0.08433905053646207</v>
-      </c>
-      <c r="AK15" t="n">
-        <v>0.1330071307243195</v>
-      </c>
-      <c r="AL15" t="n">
-        <v>-0.06554152103180577</v>
-      </c>
-      <c r="AM15" t="n">
-        <v>0.6204564520653264</v>
-      </c>
-      <c r="AN15" t="n">
-        <v>-0.1320849073694035</v>
-      </c>
-      <c r="AO15" t="n">
-        <v>1.021371496484637</v>
-      </c>
-      <c r="AP15" t="n">
-        <v>-0.05787027643081366</v>
-      </c>
-      <c r="AQ15" t="n">
-        <v>1.374983280263045</v>
-      </c>
-      <c r="AR15" t="n">
-        <v>0.1691841064615396</v>
       </c>
       <c r="AS15" t="n">
         <v>-2.283417863465212</v>
@@ -3339,42 +2811,6 @@
       </c>
       <c r="AX15" t="n">
         <v>-0.6837224190057869</v>
-      </c>
-      <c r="AY15" t="n">
-        <v>0.1219688402082357</v>
-      </c>
-      <c r="AZ15" t="n">
-        <v>0.2585811841671515</v>
-      </c>
-      <c r="BA15" t="n">
-        <v>0.2585811841671515</v>
-      </c>
-      <c r="BB15" t="n">
-        <v>-0.1407100306609759</v>
-      </c>
-      <c r="BC15" t="n">
-        <v>1.025962967106858</v>
-      </c>
-      <c r="BD15" t="n">
-        <v>-0.8360084755579631</v>
-      </c>
-      <c r="BE15" t="n">
-        <v>-0.8360084755579631</v>
-      </c>
-      <c r="BF15" t="n">
-        <v>-1.176115419189416</v>
-      </c>
-      <c r="BG15" t="n">
-        <v>-0.6837224190057869</v>
-      </c>
-      <c r="BH15" t="n">
-        <v>0.2095033587413591</v>
-      </c>
-      <c r="BI15" t="n">
-        <v>0.2095033587413591</v>
-      </c>
-      <c r="BJ15" t="n">
-        <v>0.3300031735749271</v>
       </c>
     </row>
     <row r="16">
@@ -3472,43 +2908,43 @@
         <v>44.26984178259018</v>
       </c>
       <c r="AF16" t="n">
+        <v>-0.006514914492338875</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>0.1035383407105801</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>0.05277724976235731</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>0.1751772900845161</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>0.4970504882487852</v>
+      </c>
+      <c r="AK16" t="n">
+        <v>0.1620505718474607</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>0.6585826265051082</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>-0.009565150484126761</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>0.8722908953402921</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>-0.2193382445802037</v>
+      </c>
+      <c r="AP16" t="n">
         <v>48.77119340492122</v>
       </c>
-      <c r="AG16" t="n">
+      <c r="AQ16" t="n">
         <v>66.12516409586232</v>
       </c>
-      <c r="AH16" t="n">
+      <c r="AR16" t="n">
         <v>103.9358263378644</v>
-      </c>
-      <c r="AI16" t="n">
-        <v>-0.006514914492338875</v>
-      </c>
-      <c r="AJ16" t="n">
-        <v>0.1035383407105801</v>
-      </c>
-      <c r="AK16" t="n">
-        <v>0.05277724976235731</v>
-      </c>
-      <c r="AL16" t="n">
-        <v>0.1751772900845161</v>
-      </c>
-      <c r="AM16" t="n">
-        <v>0.4970504882487852</v>
-      </c>
-      <c r="AN16" t="n">
-        <v>0.1620505718474607</v>
-      </c>
-      <c r="AO16" t="n">
-        <v>0.6585826265051082</v>
-      </c>
-      <c r="AP16" t="n">
-        <v>-0.009565150484126761</v>
-      </c>
-      <c r="AQ16" t="n">
-        <v>0.8722908953402921</v>
-      </c>
-      <c r="AR16" t="n">
-        <v>-0.2193382445802037</v>
       </c>
       <c r="AS16" t="n">
         <v>-1.559774308196062</v>
@@ -3527,42 +2963,6 @@
       </c>
       <c r="AX16" t="n">
         <v>0.06170974515061456</v>
-      </c>
-      <c r="AY16" t="n">
-        <v>0.650778460116141</v>
-      </c>
-      <c r="AZ16" t="n">
-        <v>-0.1251501885020709</v>
-      </c>
-      <c r="BA16" t="n">
-        <v>-0.1251501885020709</v>
-      </c>
-      <c r="BB16" t="n">
-        <v>-0.2658051889518074</v>
-      </c>
-      <c r="BC16" t="n">
-        <v>-0.6430711190066067</v>
-      </c>
-      <c r="BD16" t="n">
-        <v>0.796885338558234</v>
-      </c>
-      <c r="BE16" t="n">
-        <v>0.796885338558234</v>
-      </c>
-      <c r="BF16" t="n">
-        <v>0.7049876745748714</v>
-      </c>
-      <c r="BG16" t="n">
-        <v>0.06170974515061456</v>
-      </c>
-      <c r="BH16" t="n">
-        <v>1.256436966076226</v>
-      </c>
-      <c r="BI16" t="n">
-        <v>1.256436966076226</v>
-      </c>
-      <c r="BJ16" t="n">
-        <v>0.152621802606056</v>
       </c>
     </row>
     <row r="17">
@@ -3660,43 +3060,43 @@
         <v>40.55855730746655</v>
       </c>
       <c r="AF17" t="n">
+        <v>-0.05631446838379617</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>-0.07403683155140861</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>0.4055464521367504</v>
+      </c>
+      <c r="AI17" t="n">
+        <v>0.04074218425344611</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>0.7435215280411036</v>
+      </c>
+      <c r="AK17" t="n">
+        <v>-0.03224991737527638</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>1.166983868213411</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>0.1870231425508475</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>1.012964451566653</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>0.1925914845568037</v>
+      </c>
+      <c r="AP17" t="n">
         <v>46.79457888431948</v>
       </c>
-      <c r="AG17" t="n">
+      <c r="AQ17" t="n">
         <v>61.17892445190553</v>
       </c>
-      <c r="AH17" t="n">
+      <c r="AR17" t="n">
         <v>105.4521945751519</v>
-      </c>
-      <c r="AI17" t="n">
-        <v>-0.05631446838379617</v>
-      </c>
-      <c r="AJ17" t="n">
-        <v>-0.07403683155140861</v>
-      </c>
-      <c r="AK17" t="n">
-        <v>0.4055464521367504</v>
-      </c>
-      <c r="AL17" t="n">
-        <v>0.04074218425344611</v>
-      </c>
-      <c r="AM17" t="n">
-        <v>0.7435215280411036</v>
-      </c>
-      <c r="AN17" t="n">
-        <v>-0.03224991737527638</v>
-      </c>
-      <c r="AO17" t="n">
-        <v>1.166983868213411</v>
-      </c>
-      <c r="AP17" t="n">
-        <v>0.1870231425508475</v>
-      </c>
-      <c r="AQ17" t="n">
-        <v>1.012964451566653</v>
-      </c>
-      <c r="AR17" t="n">
-        <v>0.1925914845568037</v>
       </c>
       <c r="AS17" t="n">
         <v>-1.336731506935195</v>
@@ -3715,42 +3115,6 @@
       </c>
       <c r="AX17" t="n">
         <v>1.41762911973124</v>
-      </c>
-      <c r="AY17" t="n">
-        <v>0.1163673242168168</v>
-      </c>
-      <c r="AZ17" t="n">
-        <v>0.3221343487615593</v>
-      </c>
-      <c r="BA17" t="n">
-        <v>0.3221343487615593</v>
-      </c>
-      <c r="BB17" t="n">
-        <v>0.3274316336509344</v>
-      </c>
-      <c r="BC17" t="n">
-        <v>0.5078454931794143</v>
-      </c>
-      <c r="BD17" t="n">
-        <v>0.03809124902150685</v>
-      </c>
-      <c r="BE17" t="n">
-        <v>0.03809124902150685</v>
-      </c>
-      <c r="BF17" t="n">
-        <v>-0.1528595104157887</v>
-      </c>
-      <c r="BG17" t="n">
-        <v>1.41762911973124</v>
-      </c>
-      <c r="BH17" t="n">
-        <v>-1.304729204454603</v>
-      </c>
-      <c r="BI17" t="n">
-        <v>-1.304729204454603</v>
-      </c>
-      <c r="BJ17" t="n">
-        <v>-0.639648833934227</v>
       </c>
     </row>
     <row r="18">
@@ -3848,43 +3212,43 @@
         <v>37.22360083397399</v>
       </c>
       <c r="AF18" t="n">
+        <v>0.01286293597931731</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>0.0449254157695389</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>0.4359346755007465</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>0.04277939492083505</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>0.7892096296269884</v>
+      </c>
+      <c r="AK18" t="n">
+        <v>0.02938534351105204</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>1.156197710240136</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>-0.05594466594938829</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>1.171370770068876</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>-0.1802627076493888</v>
+      </c>
+      <c r="AP18" t="n">
         <v>45.28343366058499</v>
       </c>
-      <c r="AG18" t="n">
+      <c r="AQ18" t="n">
         <v>58.26406678066639</v>
       </c>
-      <c r="AH18" t="n">
+      <c r="AR18" t="n">
         <v>112.6390792913644</v>
-      </c>
-      <c r="AI18" t="n">
-        <v>0.01286293597931731</v>
-      </c>
-      <c r="AJ18" t="n">
-        <v>0.0449254157695389</v>
-      </c>
-      <c r="AK18" t="n">
-        <v>0.4359346755007465</v>
-      </c>
-      <c r="AL18" t="n">
-        <v>0.04277939492083505</v>
-      </c>
-      <c r="AM18" t="n">
-        <v>0.7892096296269884</v>
-      </c>
-      <c r="AN18" t="n">
-        <v>0.02938534351105204</v>
-      </c>
-      <c r="AO18" t="n">
-        <v>1.156197710240136</v>
-      </c>
-      <c r="AP18" t="n">
-        <v>-0.05594466594938829</v>
-      </c>
-      <c r="AQ18" t="n">
-        <v>1.171370770068876</v>
-      </c>
-      <c r="AR18" t="n">
-        <v>-0.1802627076493888</v>
       </c>
       <c r="AS18" t="n">
         <v>0.1748486893719097</v>
@@ -3903,42 +3267,6 @@
       </c>
       <c r="AX18" t="n">
         <v>0.2149531585749571</v>
-      </c>
-      <c r="AY18" t="n">
-        <v>0.8916827229212303</v>
-      </c>
-      <c r="AZ18" t="n">
-        <v>0.1602218652250347</v>
-      </c>
-      <c r="BA18" t="n">
-        <v>0.1602218652250347</v>
-      </c>
-      <c r="BB18" t="n">
-        <v>-0.2075701688385772</v>
-      </c>
-      <c r="BC18" t="n">
-        <v>1.04732406370228</v>
-      </c>
-      <c r="BD18" t="n">
-        <v>-0.1120878346309897</v>
-      </c>
-      <c r="BE18" t="n">
-        <v>-0.1120878346309897</v>
-      </c>
-      <c r="BF18" t="n">
-        <v>-0.6003170636825019</v>
-      </c>
-      <c r="BG18" t="n">
-        <v>0.2149531585749571</v>
-      </c>
-      <c r="BH18" t="n">
-        <v>0.3098846283363792</v>
-      </c>
-      <c r="BI18" t="n">
-        <v>0.3098846283363792</v>
-      </c>
-      <c r="BJ18" t="n">
-        <v>-0.3595027138423588</v>
       </c>
     </row>
     <row r="19">
@@ -4036,43 +3364,43 @@
         <v>36.67406934372922</v>
       </c>
       <c r="AF19" t="n">
+        <v>-0.1272485611286491</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>-0.07297434705369277</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>0.5951769808505425</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>0.00253509967885357</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>0.658570451939358</v>
+      </c>
+      <c r="AK19" t="n">
+        <v>-0.03286067475663401</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>0.8957588926274695</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>-0.2114917369599123</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>0.8179213138336934</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>-0.01157319292109271</v>
+      </c>
+      <c r="AP19" t="n">
         <v>47.33901932853543</v>
       </c>
-      <c r="AG19" t="n">
+      <c r="AQ19" t="n">
         <v>59.53850536423637</v>
       </c>
-      <c r="AH19" t="n">
+      <c r="AR19" t="n">
         <v>120.6857766418767</v>
-      </c>
-      <c r="AI19" t="n">
-        <v>-0.1272485611286491</v>
-      </c>
-      <c r="AJ19" t="n">
-        <v>-0.07297434705369277</v>
-      </c>
-      <c r="AK19" t="n">
-        <v>0.5951769808505425</v>
-      </c>
-      <c r="AL19" t="n">
-        <v>0.00253509967885357</v>
-      </c>
-      <c r="AM19" t="n">
-        <v>0.658570451939358</v>
-      </c>
-      <c r="AN19" t="n">
-        <v>-0.03286067475663401</v>
-      </c>
-      <c r="AO19" t="n">
-        <v>0.8957588926274695</v>
-      </c>
-      <c r="AP19" t="n">
-        <v>-0.2114917369599123</v>
-      </c>
-      <c r="AQ19" t="n">
-        <v>0.8179213138336934</v>
-      </c>
-      <c r="AR19" t="n">
-        <v>-0.01157319292109271</v>
       </c>
       <c r="AS19" t="n">
         <v>2.327316346579153</v>
@@ -4091,42 +3419,6 @@
       </c>
       <c r="AX19" t="n">
         <v>-2.425733657950761</v>
-      </c>
-      <c r="AY19" t="n">
-        <v>0.8367174462713352</v>
-      </c>
-      <c r="AZ19" t="n">
-        <v>-0.6063376801324081</v>
-      </c>
-      <c r="BA19" t="n">
-        <v>-0.6063376801324081</v>
-      </c>
-      <c r="BB19" t="n">
-        <v>-0.3818878044594626</v>
-      </c>
-      <c r="BC19" t="n">
-        <v>-0.814465620504861</v>
-      </c>
-      <c r="BD19" t="n">
-        <v>-0.4719443185595731</v>
-      </c>
-      <c r="BE19" t="n">
-        <v>-0.4719443185595731</v>
-      </c>
-      <c r="BF19" t="n">
-        <v>0.7923816366241688</v>
-      </c>
-      <c r="BG19" t="n">
-        <v>-2.425733657950761</v>
-      </c>
-      <c r="BH19" t="n">
-        <v>-0.7007346408027977</v>
-      </c>
-      <c r="BI19" t="n">
-        <v>-0.7007346408027977</v>
-      </c>
-      <c r="BJ19" t="n">
-        <v>1.577002903803111</v>
       </c>
     </row>
     <row r="20">
@@ -4224,43 +3516,43 @@
         <v>36.19005933721014</v>
       </c>
       <c r="AF20" t="n">
+        <v>-0.01945444878111502</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>0.1156152562892192</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>0.4463312473702956</v>
+      </c>
+      <c r="AI20" t="n">
+        <v>-0.001561895329903251</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>0.6789877059611875</v>
+      </c>
+      <c r="AK20" t="n">
+        <v>0.04003377670936814</v>
+      </c>
+      <c r="AL20" t="n">
+        <v>0.7838822425679908</v>
+      </c>
+      <c r="AM20" t="n">
+        <v>0.1852583377919395</v>
+      </c>
+      <c r="AN20" t="n">
+        <v>0.9407469566832098</v>
+      </c>
+      <c r="AO20" t="n">
+        <v>0.1316339411634058</v>
+      </c>
+      <c r="AP20" t="n">
         <v>52.74147478157121</v>
       </c>
-      <c r="AG20" t="n">
+      <c r="AQ20" t="n">
         <v>57.55508146578691</v>
       </c>
-      <c r="AH20" t="n">
+      <c r="AR20" t="n">
         <v>119.0295393605859</v>
-      </c>
-      <c r="AI20" t="n">
-        <v>-0.01945444878111502</v>
-      </c>
-      <c r="AJ20" t="n">
-        <v>0.1156152562892192</v>
-      </c>
-      <c r="AK20" t="n">
-        <v>0.4463312473702956</v>
-      </c>
-      <c r="AL20" t="n">
-        <v>-0.001561895329903251</v>
-      </c>
-      <c r="AM20" t="n">
-        <v>0.6789877059611875</v>
-      </c>
-      <c r="AN20" t="n">
-        <v>0.04003377670936814</v>
-      </c>
-      <c r="AO20" t="n">
-        <v>0.7838822425679908</v>
-      </c>
-      <c r="AP20" t="n">
-        <v>0.1852583377919395</v>
-      </c>
-      <c r="AQ20" t="n">
-        <v>0.9407469566832098</v>
-      </c>
-      <c r="AR20" t="n">
-        <v>0.1316339411634058</v>
       </c>
       <c r="AS20" t="n">
         <v>2.054433283256763</v>
@@ -4279,42 +3571,6 @@
       </c>
       <c r="AX20" t="n">
         <v>1.241591140735967</v>
-      </c>
-      <c r="AY20" t="n">
-        <v>-0.7457990482164103</v>
-      </c>
-      <c r="AZ20" t="n">
-        <v>-0.1263545291424484</v>
-      </c>
-      <c r="BA20" t="n">
-        <v>-0.1263545291424484</v>
-      </c>
-      <c r="BB20" t="n">
-        <v>0.6687275685202478</v>
-      </c>
-      <c r="BC20" t="n">
-        <v>0.4932712417846727</v>
-      </c>
-      <c r="BD20" t="n">
-        <v>0.3997171985847086</v>
-      </c>
-      <c r="BE20" t="n">
-        <v>0.3997171985847086</v>
-      </c>
-      <c r="BF20" t="n">
-        <v>-0.5251947537934185</v>
-      </c>
-      <c r="BG20" t="n">
-        <v>1.241591140735967</v>
-      </c>
-      <c r="BH20" t="n">
-        <v>1.100393351254233</v>
-      </c>
-      <c r="BI20" t="n">
-        <v>1.100393351254233</v>
-      </c>
-      <c r="BJ20" t="n">
-        <v>-1.491563240607305</v>
       </c>
     </row>
     <row r="21">
@@ -4412,43 +3668,43 @@
         <v>36.95487976074219</v>
       </c>
       <c r="AF21" t="n">
+        <v>0.154762572430549</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>0.03731098580867354</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>0.5900210522590754</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>0.009319376438222449</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>0.9096972485806063</v>
+      </c>
+      <c r="AK21" t="n">
+        <v>0.09031143594295976</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>1.063660865134391</v>
+      </c>
+      <c r="AM21" t="n">
+        <v>-0.0961237765373113</v>
+      </c>
+      <c r="AN21" t="n">
+        <v>1.031069045371204</v>
+      </c>
+      <c r="AO21" t="n">
+        <v>-0.1134778590912457</v>
+      </c>
+      <c r="AP21" t="n">
         <v>55.16073404174135</v>
       </c>
-      <c r="AG21" t="n">
+      <c r="AQ21" t="n">
         <v>57.54474253447614</v>
       </c>
-      <c r="AH21" t="n">
+      <c r="AR21" t="n">
         <v>122.3396666422391</v>
-      </c>
-      <c r="AI21" t="n">
-        <v>0.154762572430549</v>
-      </c>
-      <c r="AJ21" t="n">
-        <v>0.03731098580867354</v>
-      </c>
-      <c r="AK21" t="n">
-        <v>0.5900210522590754</v>
-      </c>
-      <c r="AL21" t="n">
-        <v>0.009319376438222449</v>
-      </c>
-      <c r="AM21" t="n">
-        <v>0.9096972485806063</v>
-      </c>
-      <c r="AN21" t="n">
-        <v>0.09031143594295976</v>
-      </c>
-      <c r="AO21" t="n">
-        <v>1.063660865134391</v>
-      </c>
-      <c r="AP21" t="n">
-        <v>-0.0961237765373113</v>
-      </c>
-      <c r="AQ21" t="n">
-        <v>1.031069045371204</v>
-      </c>
-      <c r="AR21" t="n">
-        <v>-0.1134778590912457</v>
       </c>
       <c r="AS21" t="n">
         <v>1.27613210336458</v>
@@ -4467,42 +3723,6 @@
       </c>
       <c r="AX21" t="n">
         <v>-1.057337023006526</v>
-      </c>
-      <c r="AY21" t="n">
-        <v>0.3465947313768356</v>
-      </c>
-      <c r="AZ21" t="n">
-        <v>0.4417156169444454</v>
-      </c>
-      <c r="BA21" t="n">
-        <v>0.4417156169444454</v>
-      </c>
-      <c r="BB21" t="n">
-        <v>-0.2177454518334778</v>
-      </c>
-      <c r="BC21" t="n">
-        <v>-0.2997709110994675</v>
-      </c>
-      <c r="BD21" t="n">
-        <v>-0.3450193890965103</v>
-      </c>
-      <c r="BE21" t="n">
-        <v>-0.3450193890965103</v>
-      </c>
-      <c r="BF21" t="n">
-        <v>0.2788612645340485</v>
-      </c>
-      <c r="BG21" t="n">
-        <v>-1.057337023006526</v>
-      </c>
-      <c r="BH21" t="n">
-        <v>-1.220784326871393</v>
-      </c>
-      <c r="BI21" t="n">
-        <v>-1.220784326871393</v>
-      </c>
-      <c r="BJ21" t="n">
-        <v>0.8133756134189249</v>
       </c>
     </row>
     <row r="22">
@@ -4600,43 +3820,43 @@
         <v>36.52777164540392</v>
       </c>
       <c r="AF22" t="n">
+        <v>0.3472835459607708</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>0.2462442885053964</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>0.6895303726196289</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>0.3981017051859101</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>0.8530028322909828</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>0.009189768040432256</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>0.7571494325678394</v>
+      </c>
+      <c r="AM22" t="n">
+        <v>0.08922764595518728</v>
+      </c>
+      <c r="AN22" t="n">
+        <v>0.9578030160132833</v>
+      </c>
+      <c r="AO22" t="n">
+        <v>0.1771209087777557</v>
+      </c>
+      <c r="AP22" t="n">
         <v>58.96637222741883</v>
       </c>
-      <c r="AG22" t="n">
+      <c r="AQ22" t="n">
         <v>56.33531995876749</v>
       </c>
-      <c r="AH22" t="n">
+      <c r="AR22" t="n">
         <v>121.4204458318661</v>
-      </c>
-      <c r="AI22" t="n">
-        <v>0.3472835459607708</v>
-      </c>
-      <c r="AJ22" t="n">
-        <v>0.2462442885053964</v>
-      </c>
-      <c r="AK22" t="n">
-        <v>0.6895303726196289</v>
-      </c>
-      <c r="AL22" t="n">
-        <v>0.3981017051859101</v>
-      </c>
-      <c r="AM22" t="n">
-        <v>0.8530028322909828</v>
-      </c>
-      <c r="AN22" t="n">
-        <v>0.009189768040432256</v>
-      </c>
-      <c r="AO22" t="n">
-        <v>0.7571494325678394</v>
-      </c>
-      <c r="AP22" t="n">
-        <v>0.08922764595518728</v>
-      </c>
-      <c r="AQ22" t="n">
-        <v>0.9578030160132833</v>
-      </c>
-      <c r="AR22" t="n">
-        <v>0.1771209087777557</v>
       </c>
       <c r="AS22" t="n">
         <v>2.264693391250179</v>
@@ -4655,42 +3875,6 @@
       </c>
       <c r="AX22" t="n">
         <v>-0.1027627330733187</v>
-      </c>
-      <c r="AY22" t="n">
-        <v>0.5680067036361702</v>
-      </c>
-      <c r="AZ22" t="n">
-        <v>0.09990003723019814</v>
-      </c>
-      <c r="BA22" t="n">
-        <v>0.09990003723019814</v>
-      </c>
-      <c r="BB22" t="n">
-        <v>-0.05569736380043289</v>
-      </c>
-      <c r="BC22" t="n">
-        <v>0.0226319941525861</v>
-      </c>
-      <c r="BD22" t="n">
-        <v>0.6322817114663069</v>
-      </c>
-      <c r="BE22" t="n">
-        <v>0.6322817114663069</v>
-      </c>
-      <c r="BF22" t="n">
-        <v>-0.07388209296339643</v>
-      </c>
-      <c r="BG22" t="n">
-        <v>-0.1027627330733187</v>
-      </c>
-      <c r="BH22" t="n">
-        <v>1.779130854921191</v>
-      </c>
-      <c r="BI22" t="n">
-        <v>1.779130854921191</v>
-      </c>
-      <c r="BJ22" t="n">
-        <v>-0.04234236802604308</v>
       </c>
     </row>
     <row r="23">
@@ -4788,43 +3972,43 @@
         <v>34.95622594305809</v>
       </c>
       <c r="AF23" t="n">
+        <v>0.8305082929895313</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>0.01708649574441878</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>1.774630648024541</v>
+      </c>
+      <c r="AI23" t="n">
+        <v>0.1818311975357467</v>
+      </c>
+      <c r="AJ23" t="n">
+        <v>1.155431219872007</v>
+      </c>
+      <c r="AK23" t="n">
+        <v>0.271213308293758</v>
+      </c>
+      <c r="AL23" t="n">
+        <v>1.327621175887732</v>
+      </c>
+      <c r="AM23" t="n">
+        <v>0.3049191008222802</v>
+      </c>
+      <c r="AN23" t="n">
+        <v>1.435184478759759</v>
+      </c>
+      <c r="AO23" t="n">
+        <v>0.106870874445498</v>
+      </c>
+      <c r="AP23" t="n">
         <v>64.11915033210836</v>
       </c>
-      <c r="AG23" t="n">
+      <c r="AQ23" t="n">
         <v>54.95394646213266</v>
       </c>
-      <c r="AH23" t="n">
+      <c r="AR23" t="n">
         <v>119.1459730191142</v>
-      </c>
-      <c r="AI23" t="n">
-        <v>0.8305082929895313</v>
-      </c>
-      <c r="AJ23" t="n">
-        <v>0.01708649574441878</v>
-      </c>
-      <c r="AK23" t="n">
-        <v>1.774630648024541</v>
-      </c>
-      <c r="AL23" t="n">
-        <v>0.1818311975357467</v>
-      </c>
-      <c r="AM23" t="n">
-        <v>1.155431219872007</v>
-      </c>
-      <c r="AN23" t="n">
-        <v>0.271213308293758</v>
-      </c>
-      <c r="AO23" t="n">
-        <v>1.327621175887732</v>
-      </c>
-      <c r="AP23" t="n">
-        <v>0.3049191008222802</v>
-      </c>
-      <c r="AQ23" t="n">
-        <v>1.435184478759759</v>
-      </c>
-      <c r="AR23" t="n">
-        <v>0.106870874445498</v>
       </c>
       <c r="AS23" t="n">
         <v>3.795689941161952</v>
@@ -4843,42 +4027,6 @@
       </c>
       <c r="AX23" t="n">
         <v>1.173253109288212</v>
-      </c>
-      <c r="AY23" t="n">
-        <v>0.7797305254835303</v>
-      </c>
-      <c r="AZ23" t="n">
-        <v>-0.1573516358399702</v>
-      </c>
-      <c r="BA23" t="n">
-        <v>-0.1573516358399702</v>
-      </c>
-      <c r="BB23" t="n">
-        <v>-0.1667443997165097</v>
-      </c>
-      <c r="BC23" t="n">
-        <v>0.7061687311585838</v>
-      </c>
-      <c r="BD23" t="n">
-        <v>-0.4912483796973774</v>
-      </c>
-      <c r="BE23" t="n">
-        <v>-0.4912483796973774</v>
-      </c>
-      <c r="BF23" t="n">
-        <v>-0.6356080579986062</v>
-      </c>
-      <c r="BG23" t="n">
-        <v>1.173253109288212</v>
-      </c>
-      <c r="BH23" t="n">
-        <v>-0.2077130053066267</v>
-      </c>
-      <c r="BI23" t="n">
-        <v>-0.2077130053066267</v>
-      </c>
-      <c r="BJ23" t="n">
-        <v>-0.5020115853115292</v>
       </c>
     </row>
     <row r="24">
@@ -4976,43 +4124,43 @@
         <v>34.86377431991254</v>
       </c>
       <c r="AF24" t="n">
+        <v>0.4760823351271597</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>-0.1017616150227045</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>1.392113908808295</v>
+      </c>
+      <c r="AI24" t="n">
+        <v>0.008468932293826725</v>
+      </c>
+      <c r="AJ24" t="n">
+        <v>1.434350521006468</v>
+      </c>
+      <c r="AK24" t="n">
+        <v>0.2164252260898039</v>
+      </c>
+      <c r="AL24" t="n">
+        <v>1.551581443624286</v>
+      </c>
+      <c r="AM24" t="n">
+        <v>0.2455701219274697</v>
+      </c>
+      <c r="AN24" t="n">
+        <v>1.301344404829315</v>
+      </c>
+      <c r="AO24" t="n">
+        <v>0.03689705057347403</v>
+      </c>
+      <c r="AP24" t="n">
         <v>69.85140906166851</v>
       </c>
-      <c r="AG24" t="n">
+      <c r="AQ24" t="n">
         <v>55.99252282493386</v>
       </c>
-      <c r="AH24" t="n">
+      <c r="AR24" t="n">
         <v>121.6886553317583</v>
-      </c>
-      <c r="AI24" t="n">
-        <v>0.4760823351271597</v>
-      </c>
-      <c r="AJ24" t="n">
-        <v>-0.1017616150227045</v>
-      </c>
-      <c r="AK24" t="n">
-        <v>1.392113908808295</v>
-      </c>
-      <c r="AL24" t="n">
-        <v>0.008468932293826725</v>
-      </c>
-      <c r="AM24" t="n">
-        <v>1.434350521006468</v>
-      </c>
-      <c r="AN24" t="n">
-        <v>0.2164252260898039</v>
-      </c>
-      <c r="AO24" t="n">
-        <v>1.551581443624286</v>
-      </c>
-      <c r="AP24" t="n">
-        <v>0.2455701219274697</v>
-      </c>
-      <c r="AQ24" t="n">
-        <v>1.301344404829315</v>
-      </c>
-      <c r="AR24" t="n">
-        <v>0.03689705057347403</v>
       </c>
       <c r="AS24" t="n">
         <v>4.346275436079073</v>
@@ -5031,42 +4179,6 @@
       </c>
       <c r="AX24" t="n">
         <v>2.071085526627386</v>
-      </c>
-      <c r="AY24" t="n">
-        <v>0.5659446940882402</v>
-      </c>
-      <c r="AZ24" t="n">
-        <v>-0.05720862866066612</v>
-      </c>
-      <c r="BA24" t="n">
-        <v>-0.05720862866066612</v>
-      </c>
-      <c r="BB24" t="n">
-        <v>0.1654348520359248</v>
-      </c>
-      <c r="BC24" t="n">
-        <v>0.4968737454237084</v>
-      </c>
-      <c r="BD24" t="n">
-        <v>-0.4932897285084459</v>
-      </c>
-      <c r="BE24" t="n">
-        <v>-0.4932897285084459</v>
-      </c>
-      <c r="BF24" t="n">
-        <v>-0.305062102946999</v>
-      </c>
-      <c r="BG24" t="n">
-        <v>2.071085526627386</v>
-      </c>
-      <c r="BH24" t="n">
-        <v>-0.3655727995106957</v>
-      </c>
-      <c r="BI24" t="n">
-        <v>-0.3655727995106957</v>
-      </c>
-      <c r="BJ24" t="n">
-        <v>-1.240602262180038</v>
       </c>
     </row>
     <row r="25">
@@ -5164,43 +4276,43 @@
         <v>36.08174831309217</v>
       </c>
       <c r="AF25" t="n">
+        <v>0.6314510994769122</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>0.1651479842815</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>1.726219501901177</v>
+      </c>
+      <c r="AI25" t="n">
+        <v>0.2858613399749075</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>1.856941872454705</v>
+      </c>
+      <c r="AK25" t="n">
+        <v>0.4656619213997217</v>
+      </c>
+      <c r="AL25" t="n">
+        <v>1.883954190193343</v>
+      </c>
+      <c r="AM25" t="n">
+        <v>0.3085734996389888</v>
+      </c>
+      <c r="AN25" t="n">
+        <v>1.560623087781543</v>
+      </c>
+      <c r="AO25" t="n">
+        <v>0.2411177817811385</v>
+      </c>
+      <c r="AP25" t="n">
         <v>75.9623009094794</v>
       </c>
-      <c r="AG25" t="n">
+      <c r="AQ25" t="n">
         <v>57.55243900759669</v>
       </c>
-      <c r="AH25" t="n">
+      <c r="AR25" t="n">
         <v>125.9088958545611</v>
-      </c>
-      <c r="AI25" t="n">
-        <v>0.6314510994769122</v>
-      </c>
-      <c r="AJ25" t="n">
-        <v>0.1651479842815</v>
-      </c>
-      <c r="AK25" t="n">
-        <v>1.726219501901177</v>
-      </c>
-      <c r="AL25" t="n">
-        <v>0.2858613399749075</v>
-      </c>
-      <c r="AM25" t="n">
-        <v>1.856941872454705</v>
-      </c>
-      <c r="AN25" t="n">
-        <v>0.4656619213997217</v>
-      </c>
-      <c r="AO25" t="n">
-        <v>1.883954190193343</v>
-      </c>
-      <c r="AP25" t="n">
-        <v>0.3085734996389888</v>
-      </c>
-      <c r="AQ25" t="n">
-        <v>1.560623087781543</v>
-      </c>
-      <c r="AR25" t="n">
-        <v>0.2411177817811385</v>
       </c>
       <c r="AS25" t="n">
         <v>5.509810751511417</v>
@@ -5219,42 +4331,6 @@
       </c>
       <c r="AX25" t="n">
         <v>-0.3000211377479953</v>
-      </c>
-      <c r="AY25" t="n">
-        <v>0.781017735818768</v>
-      </c>
-      <c r="AZ25" t="n">
-        <v>0.04670781060286533</v>
-      </c>
-      <c r="BA25" t="n">
-        <v>0.04670781060286533</v>
-      </c>
-      <c r="BB25" t="n">
-        <v>-0.006337353266682388</v>
-      </c>
-      <c r="BC25" t="n">
-        <v>-0.4513505257625523</v>
-      </c>
-      <c r="BD25" t="n">
-        <v>-0.6353431301385113</v>
-      </c>
-      <c r="BE25" t="n">
-        <v>-0.6353431301385113</v>
-      </c>
-      <c r="BF25" t="n">
-        <v>0.5050855058792536</v>
-      </c>
-      <c r="BG25" t="n">
-        <v>-0.3000211377479953</v>
-      </c>
-      <c r="BH25" t="n">
-        <v>-1.079888431447917</v>
-      </c>
-      <c r="BI25" t="n">
-        <v>-1.079888431447917</v>
-      </c>
-      <c r="BJ25" t="n">
-        <v>1.020812686905545</v>
       </c>
     </row>
     <row r="26">
@@ -5352,43 +4428,43 @@
         <v>36.72155826649768</v>
       </c>
       <c r="AF26" t="n">
+        <v>0.7495027907351215</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>0.1180516912582092</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>2.003935550121554</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>0.2777160482203769</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>2.282858909444627</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>0.4259170369899223</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>2.228909350456078</v>
+      </c>
+      <c r="AM26" t="n">
+        <v>0.3449551602627352</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>1.810201685479356</v>
+      </c>
+      <c r="AO26" t="n">
+        <v>0.2495785976978127</v>
+      </c>
+      <c r="AP26" t="n">
         <v>82.13830783641866</v>
       </c>
-      <c r="AG26" t="n">
+      <c r="AQ26" t="n">
         <v>57.91883823234213</v>
       </c>
-      <c r="AH26" t="n">
+      <c r="AR26" t="n">
         <v>129.0979427961256</v>
-      </c>
-      <c r="AI26" t="n">
-        <v>0.7495027907351215</v>
-      </c>
-      <c r="AJ26" t="n">
-        <v>0.1180516912582092</v>
-      </c>
-      <c r="AK26" t="n">
-        <v>2.003935550121554</v>
-      </c>
-      <c r="AL26" t="n">
-        <v>0.2777160482203769</v>
-      </c>
-      <c r="AM26" t="n">
-        <v>2.282858909444627</v>
-      </c>
-      <c r="AN26" t="n">
-        <v>0.4259170369899223</v>
-      </c>
-      <c r="AO26" t="n">
-        <v>2.228909350456078</v>
-      </c>
-      <c r="AP26" t="n">
-        <v>0.3449551602627352</v>
-      </c>
-      <c r="AQ26" t="n">
-        <v>1.810201685479356</v>
-      </c>
-      <c r="AR26" t="n">
-        <v>0.2495785976978127</v>
       </c>
       <c r="AS26" t="n">
         <v>6.176006926939266</v>
@@ -5407,42 +4483,6 @@
       </c>
       <c r="AX26" t="n">
         <v>0.2191710949542625</v>
-      </c>
-      <c r="AY26" t="n">
-        <v>0.6661961754278494</v>
-      </c>
-      <c r="AZ26" t="n">
-        <v>-0.1148215603909186</v>
-      </c>
-      <c r="BA26" t="n">
-        <v>-0.1148215603909186</v>
-      </c>
-      <c r="BB26" t="n">
-        <v>-0.1615293709937839</v>
-      </c>
-      <c r="BC26" t="n">
-        <v>-0.3700951915560964</v>
-      </c>
-      <c r="BD26" t="n">
-        <v>0.08125533420645592</v>
-      </c>
-      <c r="BE26" t="n">
-        <v>0.08125533420645592</v>
-      </c>
-      <c r="BF26" t="n">
-        <v>0.7165984643449672</v>
-      </c>
-      <c r="BG26" t="n">
-        <v>0.2191710949542625</v>
-      </c>
-      <c r="BH26" t="n">
-        <v>0.5191922327022578</v>
-      </c>
-      <c r="BI26" t="n">
-        <v>0.5191922327022578</v>
-      </c>
-      <c r="BJ26" t="n">
-        <v>1.599080664150175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>